<commit_message>
AA - Update: complete support_trascodifiche.xlsx
added all extra sheets
</commit_message>
<xml_diff>
--- a/inputs/support_trascodifiche.xlsx
+++ b/inputs/support_trascodifiche.xlsx
@@ -8,15 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://innovationteam-my.sharepoint.com/personal/a_abraham_innovationteam_eu/Documents/Documenti/progetti/22p11_Tool_FA/inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8C9F2755-18BA-4CE9-90D7-E32768AE5E81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="21" documentId="8_{8C9F2755-18BA-4CE9-90D7-E32768AE5E81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{46DABB9F-EBF8-4667-8EA8-068A47AE97FE}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15675" activeTab="2" xr2:uid="{9758A490-5BBA-4DAE-A128-35FF12EB83CB}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15675" xr2:uid="{9758A490-5BBA-4DAE-A128-35FF12EB83CB}"/>
   </bookViews>
   <sheets>
-    <sheet name="Trascodifica_Analitico_Bdgt_Eco" sheetId="2" r:id="rId1"/>
-    <sheet name="Trascodifica_Condizioni_comm_li" sheetId="3" r:id="rId2"/>
-    <sheet name="Trascodifica_CdC" sheetId="4" r:id="rId3"/>
-    <sheet name="Trascodifica_Costo_Personale" sheetId="1" r:id="rId4"/>
+    <sheet name="Condizioni_Commerciali" sheetId="7" r:id="rId1"/>
+    <sheet name="Aliquota" sheetId="6" r:id="rId2"/>
+    <sheet name="Esportatori" sheetId="8" r:id="rId3"/>
+    <sheet name="Tipo_Cliente" sheetId="5" r:id="rId4"/>
+    <sheet name="Trascodifica_Analitico_Bdgt_Eco" sheetId="2" r:id="rId5"/>
+    <sheet name="Trascodifica_Condizioni_comm_li" sheetId="3" r:id="rId6"/>
+    <sheet name="Trascodifica_CdC" sheetId="4" r:id="rId7"/>
+    <sheet name="Trascodifica_Costo_Personale" sheetId="1" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="614" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="806" uniqueCount="254">
   <si>
     <t>$CON: Codice e descrizione</t>
   </si>
@@ -539,13 +543,299 @@
   </si>
   <si>
     <t>3SERV_IT</t>
+  </si>
+  <si>
+    <t>Soggetto</t>
+  </si>
+  <si>
+    <t>Descrizione</t>
+  </si>
+  <si>
+    <t>Tipo cliente</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ROBERTO INDUSTRIA ALIMENTARE  S.R.L </t>
+  </si>
+  <si>
+    <t>Top cliente Groupage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PARMAREGGIO S.P.A. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ATLANTE S.R.L. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">PADANIA ALIMENTI S.R.L. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">CO.IND SOCIETA' COOPERATIVA </t>
+  </si>
+  <si>
+    <t xml:space="preserve">MANUZZI IMPORT EXPORT SRL </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ALIMENTA PRODUZIONI S.R.L. </t>
+  </si>
+  <si>
+    <t>COOP ALLEANZA 3.0 SOC.COOP.</t>
+  </si>
+  <si>
+    <t>Top cliente Trasporto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CENTRALE ADRIATICA SOC.COOP. </t>
+  </si>
+  <si>
+    <t>F34F43</t>
+  </si>
+  <si>
+    <t>Ragione sociale</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">IVA MEDIA </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>(2021)</t>
+    </r>
+  </si>
+  <si>
+    <t>HOVA FINE FOODS APS</t>
+  </si>
+  <si>
+    <t>COOP.AGRICOLA BRACCIANTI G.BELLINI</t>
+  </si>
+  <si>
+    <t>SARDAFORMAGGI S.P.A</t>
+  </si>
+  <si>
+    <t>MOLINI PIVETTI S.P.A</t>
+  </si>
+  <si>
+    <t>C.A.MAR SOC. COOPERATIVA</t>
+  </si>
+  <si>
+    <t>DECO INDUSTRIE S.C.P.A.</t>
+  </si>
+  <si>
+    <t>VITICOLTORI FRIULANI         *LA DE</t>
+  </si>
+  <si>
+    <t>FRIULVINI SOCIETA'COOPERATIVA AGRIC</t>
+  </si>
+  <si>
+    <t>22,0%</t>
+  </si>
+  <si>
+    <t>FURLANINA  SNC               *</t>
+  </si>
+  <si>
+    <t>MAGRI' S.R.L.</t>
+  </si>
+  <si>
+    <t>CENTRO LATTE BRESSANONE SOC.AGR.COO</t>
+  </si>
+  <si>
+    <t>I.C.A. DI ENNIO ARGIOLAS SRL</t>
+  </si>
+  <si>
+    <t>LATTERIA SOCIALE MERANO SOC.AGR.COO</t>
+  </si>
+  <si>
+    <t>CANTINE RIUNITE &amp; CIV SOC.COOP.AGR.</t>
+  </si>
+  <si>
+    <t>DISTILLERIA TURCHETTO DI ALESSANDRO</t>
+  </si>
+  <si>
+    <t>CO.PRO.PA SCARL</t>
+  </si>
+  <si>
+    <t>C.D.D. S.P.A.</t>
+  </si>
+  <si>
+    <t>SALUMIFICIO MONPIU' SRL</t>
+  </si>
+  <si>
+    <t>BRAZZALE S.P.A.</t>
+  </si>
+  <si>
+    <t>LEONCINI PROSCIUTTI S.P.A.</t>
+  </si>
+  <si>
+    <t>CONSORZIO GRANTERRE S.C.A.</t>
+  </si>
+  <si>
+    <t>COOPERATIVA CARTAI MODENESE SOC.COO</t>
+  </si>
+  <si>
+    <t>C.S.C. SOCIETA' COOPERATIVA</t>
+  </si>
+  <si>
+    <t>ROBERTO INDUSTRIA ALIMENTARE  S.R.L</t>
+  </si>
+  <si>
+    <t>EURIAL ITALIA SPA CON SOCIO UNICO</t>
+  </si>
+  <si>
+    <t>DELICIUS RIZZOLI S.P.A.</t>
+  </si>
+  <si>
+    <t>MONARI FEDERZONI SPA</t>
+  </si>
+  <si>
+    <t>CESARE REGNOLI &amp; FIGLIO S.R.L.</t>
+  </si>
+  <si>
+    <t>COOPSERVICE S.COOP.P.A.</t>
+  </si>
+  <si>
+    <t>C.R.M. SPA</t>
+  </si>
+  <si>
+    <t>COLLA S.P.A.</t>
+  </si>
+  <si>
+    <t>SALUMIFICIO SAN MICHELE S.P.A.</t>
+  </si>
+  <si>
+    <t>ALINOR S.P.A.</t>
+  </si>
+  <si>
+    <t>BONI S.P.A</t>
+  </si>
+  <si>
+    <t>INPA S.P.A.</t>
+  </si>
+  <si>
+    <t>OR.V.A. S.R.L.</t>
+  </si>
+  <si>
+    <t>RANDI SNC DI RANDI DENNIS E C.</t>
+  </si>
+  <si>
+    <t>BIRAGHI S.P.A.</t>
+  </si>
+  <si>
+    <t>FELSINEO SPA</t>
+  </si>
+  <si>
+    <t>CO.IND SOCIETA' COOPERATIVA</t>
+  </si>
+  <si>
+    <t>Ter_descr</t>
+  </si>
+  <si>
+    <t>ALCE NERO S.P.A.</t>
+  </si>
+  <si>
+    <t>ALIMENTA PRODUZIONI S.R.L.</t>
+  </si>
+  <si>
+    <t>AMBROSI S.P.A.</t>
+  </si>
+  <si>
+    <t>BIA S.P.A.</t>
+  </si>
+  <si>
+    <t>BOUVARD ITALIA SPA</t>
+  </si>
+  <si>
+    <t>BRENDOLAN SERVICE S.R.L.UNIPERSONALE</t>
+  </si>
+  <si>
+    <t>BUONA COMPAGNIA GOURMET SRL</t>
+  </si>
+  <si>
+    <t>CEREAL FOOD SRL</t>
+  </si>
+  <si>
+    <t>CILENTO S.P.A.</t>
+  </si>
+  <si>
+    <t>CONAPI SOC.COOP.</t>
+  </si>
+  <si>
+    <t>DOLCIARIA ROVELLI S.R.L.</t>
+  </si>
+  <si>
+    <t>EUROPI S.R.L</t>
+  </si>
+  <si>
+    <t>FINE FOODS &amp; PHARMACEUTICAL N.T.M</t>
+  </si>
+  <si>
+    <t>GENNARO AURICCHIO SPA</t>
+  </si>
+  <si>
+    <t>INALPI S.P.A.</t>
+  </si>
+  <si>
+    <t>ONE FOOD S.R.L.</t>
+  </si>
+  <si>
+    <t>PARMAREGGIO S.P.A.</t>
+  </si>
+  <si>
+    <t>RO.MAR. S.R.L</t>
+  </si>
+  <si>
+    <t>SOLO COSE BUONE SRL</t>
+  </si>
+  <si>
+    <t>VILLA DEGLI OLMI S.P.A.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Condizioni di pagamento </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>(2021)</t>
+    </r>
+  </si>
+  <si>
+    <t>CAVANI MASSIMO</t>
+  </si>
+  <si>
+    <t>GAITA ANTONIO</t>
+  </si>
+  <si>
+    <t>AUTOSERVIZI BIZZARRO S.P.A.</t>
+  </si>
+  <si>
+    <t>CONSAR SERVICE SOC COOP</t>
+  </si>
+  <si>
+    <t>CONS.COOP.FINANZ. PER LO SVILUPPO S</t>
+  </si>
+  <si>
+    <t>BON.BANC.VISTA FATT</t>
+  </si>
+  <si>
+    <t>M.A. GRENDI DAL 1828 S.P.A.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0%"/>
+  </numFmts>
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -589,8 +879,34 @@
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -608,8 +924,14 @@
         <fgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor theme="4"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -632,12 +954,44 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="4"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="4"/>
+      </right>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -650,12 +1004,93 @@
     <xf numFmtId="49" fontId="6" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
     <cellStyle name="Normale 2" xfId="1" xr:uid="{3D0E86AB-4D3C-45D0-B0FD-4FA2CF8A5195}"/>
+    <cellStyle name="Normale 7" xfId="2" xr:uid="{53EBC274-2193-4F8D-84F3-098F077B8327}"/>
   </cellStyles>
-  <dxfs count="11">
+  <dxfs count="15">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -847,22 +1282,7 @@
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <font>
@@ -902,36 +1322,59 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{E832CCEC-F5F5-42D8-8383-1933DC5C8C1D}" name="Trascodifica_Analitico_CE" displayName="Trascodifica_Analitico_CE" ref="A1:F108" totalsRowShown="0" headerRowDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{A4B5F73C-8C81-4BA0-9486-D78D8D2EDA32}" name="Elenco_Esportatori" displayName="Elenco_Esportatori" ref="A1:B29" totalsRowShown="0" headerRowDxfId="1" headerRowCellStyle="Normale 7" dataCellStyle="Normale 7">
+  <autoFilter ref="A1:B29" xr:uid="{A4B5F73C-8C81-4BA0-9486-D78D8D2EDA32}"/>
+  <tableColumns count="2">
+    <tableColumn id="3" xr3:uid="{B1F89080-23D9-46D2-A0A2-ECC915269C09}" name="Soggetto" dataDxfId="0" dataCellStyle="Normale 7"/>
+    <tableColumn id="2" xr3:uid="{6CE5CCEB-2876-4548-B4E6-7A22BC4AC5CA}" name="Ter_descr" dataCellStyle="Normale 7"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{A4CD4984-42E8-4E8F-9C29-4F867B1919A0}" name="Top_Clienti" displayName="Top_Clienti" ref="A1:C11" totalsRowShown="0" headerRowDxfId="14">
+  <autoFilter ref="A1:C11" xr:uid="{A4CD4984-42E8-4E8F-9C29-4F867B1919A0}"/>
+  <tableColumns count="3">
+    <tableColumn id="4" xr3:uid="{6AAC45EB-A00C-459D-8C5B-AC959ABE7DCD}" name="Soggetto" dataDxfId="13"/>
+    <tableColumn id="2" xr3:uid="{7B6BFE59-FA92-466B-995F-DD6BD01640AB}" name="Descrizione"/>
+    <tableColumn id="3" xr3:uid="{2088016D-F766-4701-8F36-DF5294CD2639}" name="Tipo cliente"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{E832CCEC-F5F5-42D8-8383-1933DC5C8C1D}" name="Trascodifica_Analitico_CE" displayName="Trascodifica_Analitico_CE" ref="A1:F108" totalsRowShown="0" headerRowDxfId="12">
   <autoFilter ref="A1:F108" xr:uid="{E832CCEC-F5F5-42D8-8383-1933DC5C8C1D}"/>
   <tableColumns count="6">
-    <tableColumn id="3" xr3:uid="{EDD3DE90-20FA-4C95-8697-6D0CFBD3D34A}" name="Chiave trascodifica" dataDxfId="7">
+    <tableColumn id="3" xr3:uid="{EDD3DE90-20FA-4C95-8697-6D0CFBD3D34A}" name="Chiave trascodifica" dataDxfId="11">
       <calculatedColumnFormula>+B2&amp;C2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="1" xr3:uid="{DB9DB5AC-9FF8-4926-8033-21AB8F0B4EFD}" name="$CDC: RAGGRUPPAMENTI_adj" dataDxfId="6"/>
+    <tableColumn id="1" xr3:uid="{DB9DB5AC-9FF8-4926-8033-21AB8F0B4EFD}" name="$CDC: RAGGRUPPAMENTI_adj" dataDxfId="10"/>
     <tableColumn id="2" xr3:uid="{06FBF0B0-A15D-4AFB-B465-7242820CF73D}" name="$CON: UNLG - Liv. 2"/>
-    <tableColumn id="4" xr3:uid="{794FE058-6F00-44B3-9FCF-51AA95F79206}" name="Trascodifica" dataDxfId="5"/>
-    <tableColumn id="5" xr3:uid="{DE8BD87C-828E-4931-A2F6-80DEA4839364}" name="Tipo voce" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{794FE058-6F00-44B3-9FCF-51AA95F79206}" name="Trascodifica" dataDxfId="9"/>
+    <tableColumn id="5" xr3:uid="{DE8BD87C-828E-4931-A2F6-80DEA4839364}" name="Tipo voce" dataDxfId="8"/>
     <tableColumn id="6" xr3:uid="{D7A74A4A-9FFA-42A1-A081-4618874B9909}" name="Note"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
-<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{18C42134-E9F8-4487-A759-0E0A55C87CC7}" name="Trascodifica_Condizioni_Commerciali" displayName="Trascodifica_Condizioni_Commerciali" ref="A1:C23" totalsRowShown="0" headerRowDxfId="3">
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{18C42134-E9F8-4487-A759-0E0A55C87CC7}" name="Trascodifica_Condizioni_Commerciali" displayName="Trascodifica_Condizioni_Commerciali" ref="A1:C23" totalsRowShown="0" headerRowDxfId="7">
   <autoFilter ref="A1:C23" xr:uid="{18C42134-E9F8-4487-A759-0E0A55C87CC7}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{EEC8624E-B158-4B11-8B15-87315EDB7A65}" name="Condizioni commerciali nominali"/>
-    <tableColumn id="2" xr3:uid="{0E26CAB4-E054-46FC-9425-1C33322A5A5F}" name="Condizioni commerciali nominali_riclassificato" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{F50EB424-39EE-40F9-9560-3D7FF968902F}" name="Modalità pagamento" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{0E26CAB4-E054-46FC-9425-1C33322A5A5F}" name="Condizioni commerciali nominali_riclassificato" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{F50EB424-39EE-40F9-9560-3D7FF968902F}" name="Modalità pagamento" dataDxfId="5"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
-<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{3A8FC088-1845-4A45-A33F-B35A68332615}" name="Trascodifica_CdC" displayName="Trascodifica_CdC" ref="A1:B13" totalsRowShown="0" headerRowDxfId="0" headerRowCellStyle="Normale 2" dataCellStyle="Normale 2">
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{3A8FC088-1845-4A45-A33F-B35A68332615}" name="Trascodifica_CdC" displayName="Trascodifica_CdC" ref="A1:B13" totalsRowShown="0" headerRowDxfId="4" headerRowCellStyle="Normale 2" dataCellStyle="Normale 2">
   <autoFilter ref="A1:B13" xr:uid="{3A8FC088-1845-4A45-A33F-B35A68332615}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{7EA54190-3906-4667-AA7A-4FC8279040CA}" name="$CDC: RAGGRUPPAMENTI " dataCellStyle="Normale 2"/>
@@ -941,12 +1384,12 @@
 </table>
 </file>
 
-<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{42411417-7B51-4A46-A8D2-79D3CB8FE77A}" name="Trascodifica_Costo_Personale" displayName="Trascodifica_Costo_Personale" ref="A1:B39" totalsRowShown="0" headerRowDxfId="10">
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{42411417-7B51-4A46-A8D2-79D3CB8FE77A}" name="Trascodifica_Costo_Personale" displayName="Trascodifica_Costo_Personale" ref="A1:B39" totalsRowShown="0" headerRowDxfId="3">
   <autoFilter ref="A1:B39" xr:uid="{42411417-7B51-4A46-A8D2-79D3CB8FE77A}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{41908B3F-CDCD-4896-B2C7-8E40BD4D38AA}" name="$CON: Codice e descrizione"/>
-    <tableColumn id="2" xr3:uid="{1BD768D9-BD65-4B3D-B940-62522AAB9168}" name="Tipo costo" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{1BD768D9-BD65-4B3D-B940-62522AAB9168}" name="Tipo costo" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1248,6 +1691,1401 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8A799A3-2DEF-4D6D-A2E7-3FD643717F06}">
+  <dimension ref="A1:C47"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G30" sqref="G30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.73046875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.9296875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A1" s="10" t="s">
+        <v>167</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>182</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A2" s="13">
+        <v>17</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>247</v>
+      </c>
+      <c r="C2" s="18" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A3" s="13">
+        <v>25</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>184</v>
+      </c>
+      <c r="C3" s="18" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A4" s="13">
+        <v>40</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>248</v>
+      </c>
+      <c r="C4" s="18" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A5" s="13">
+        <v>78</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>185</v>
+      </c>
+      <c r="C5" s="18" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A6" s="13">
+        <v>79</v>
+      </c>
+      <c r="B6" s="14" t="s">
+        <v>186</v>
+      </c>
+      <c r="C6" s="18" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A7" s="13">
+        <v>81</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>249</v>
+      </c>
+      <c r="C7" s="18" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A8" s="13">
+        <v>83</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>187</v>
+      </c>
+      <c r="C8" s="18" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A9" s="13">
+        <v>84</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>188</v>
+      </c>
+      <c r="C9" s="18" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A10" s="13">
+        <v>89</v>
+      </c>
+      <c r="B10" s="14" t="s">
+        <v>189</v>
+      </c>
+      <c r="C10" s="18" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A11" s="13">
+        <v>92</v>
+      </c>
+      <c r="B11" s="14" t="s">
+        <v>190</v>
+      </c>
+      <c r="C11" s="18" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A12" s="13">
+        <v>93</v>
+      </c>
+      <c r="B12" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="C12" s="18" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A13" s="13">
+        <v>95</v>
+      </c>
+      <c r="B13" s="14" t="s">
+        <v>250</v>
+      </c>
+      <c r="C13" s="18" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A14" s="13">
+        <v>98</v>
+      </c>
+      <c r="B14" s="14" t="s">
+        <v>193</v>
+      </c>
+      <c r="C14" s="18" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A15" s="13">
+        <v>99</v>
+      </c>
+      <c r="B15" s="14" t="s">
+        <v>194</v>
+      </c>
+      <c r="C15" s="18" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A16" s="13">
+        <v>102</v>
+      </c>
+      <c r="B16" s="14" t="s">
+        <v>195</v>
+      </c>
+      <c r="C16" s="18" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A17" s="13">
+        <v>104</v>
+      </c>
+      <c r="B17" s="14" t="s">
+        <v>196</v>
+      </c>
+      <c r="C17" s="18" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A18" s="13">
+        <v>105</v>
+      </c>
+      <c r="B18" s="14" t="s">
+        <v>197</v>
+      </c>
+      <c r="C18" s="18" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A19" s="13">
+        <v>118</v>
+      </c>
+      <c r="B19" s="14" t="s">
+        <v>198</v>
+      </c>
+      <c r="C19" s="18" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A20" s="13">
+        <v>121</v>
+      </c>
+      <c r="B20" s="14" t="s">
+        <v>251</v>
+      </c>
+      <c r="C20" s="18" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A21" s="13">
+        <v>122</v>
+      </c>
+      <c r="B21" s="14" t="s">
+        <v>199</v>
+      </c>
+      <c r="C21" s="18" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A22" s="13">
+        <v>128</v>
+      </c>
+      <c r="B22" s="14" t="s">
+        <v>253</v>
+      </c>
+      <c r="C22" s="18" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A23" s="13">
+        <v>139</v>
+      </c>
+      <c r="B23" s="14" t="s">
+        <v>200</v>
+      </c>
+      <c r="C23" s="18" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A24" s="13">
+        <v>141</v>
+      </c>
+      <c r="B24" s="14" t="s">
+        <v>201</v>
+      </c>
+      <c r="C24" s="18" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A25" s="13">
+        <v>145</v>
+      </c>
+      <c r="B25" s="14" t="s">
+        <v>202</v>
+      </c>
+      <c r="C25" s="18" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A26" s="13">
+        <v>146</v>
+      </c>
+      <c r="B26" s="14" t="s">
+        <v>203</v>
+      </c>
+      <c r="C26" s="18" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A27" s="13">
+        <v>147</v>
+      </c>
+      <c r="B27" s="14" t="s">
+        <v>204</v>
+      </c>
+      <c r="C27" s="18" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A28" s="13">
+        <v>150</v>
+      </c>
+      <c r="B28" s="14" t="s">
+        <v>205</v>
+      </c>
+      <c r="C28" s="18" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A29" s="13">
+        <v>160</v>
+      </c>
+      <c r="B29" s="14" t="s">
+        <v>206</v>
+      </c>
+      <c r="C29" s="18" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A30" s="13">
+        <v>164</v>
+      </c>
+      <c r="B30" s="14" t="s">
+        <v>207</v>
+      </c>
+      <c r="C30" s="18" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A31" s="13">
+        <v>178</v>
+      </c>
+      <c r="B31" s="14" t="s">
+        <v>208</v>
+      </c>
+      <c r="C31" s="18" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A32" s="13">
+        <v>182</v>
+      </c>
+      <c r="B32" s="14" t="s">
+        <v>209</v>
+      </c>
+      <c r="C32" s="18" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A33" s="13">
+        <v>210</v>
+      </c>
+      <c r="B33" s="14" t="s">
+        <v>210</v>
+      </c>
+      <c r="C33" s="18" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A34" s="13">
+        <v>220</v>
+      </c>
+      <c r="B34" s="14" t="s">
+        <v>211</v>
+      </c>
+      <c r="C34" s="18" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A35" s="13">
+        <v>228</v>
+      </c>
+      <c r="B35" s="14" t="s">
+        <v>212</v>
+      </c>
+      <c r="C35" s="18" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A36" s="13">
+        <v>235</v>
+      </c>
+      <c r="B36" s="14" t="s">
+        <v>213</v>
+      </c>
+      <c r="C36" s="18" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A37" s="13">
+        <v>245</v>
+      </c>
+      <c r="B37" s="14" t="s">
+        <v>214</v>
+      </c>
+      <c r="C37" s="18" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A38" s="13">
+        <v>250</v>
+      </c>
+      <c r="B38" s="14" t="s">
+        <v>215</v>
+      </c>
+      <c r="C38" s="18" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A39" s="13">
+        <v>256</v>
+      </c>
+      <c r="B39" s="14" t="s">
+        <v>216</v>
+      </c>
+      <c r="C39" s="18" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A40" s="13">
+        <v>263</v>
+      </c>
+      <c r="B40" s="14" t="s">
+        <v>217</v>
+      </c>
+      <c r="C40" s="18" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A41" s="13">
+        <v>272</v>
+      </c>
+      <c r="B41" s="14" t="s">
+        <v>218</v>
+      </c>
+      <c r="C41" s="18" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A42" s="13">
+        <v>278</v>
+      </c>
+      <c r="B42" s="14" t="s">
+        <v>219</v>
+      </c>
+      <c r="C42" s="18" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A43" s="13">
+        <v>290</v>
+      </c>
+      <c r="B43" s="14" t="s">
+        <v>220</v>
+      </c>
+      <c r="C43" s="18" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A44" s="13">
+        <v>291</v>
+      </c>
+      <c r="B44" s="14" t="s">
+        <v>221</v>
+      </c>
+      <c r="C44" s="18" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A45" s="13">
+        <v>292</v>
+      </c>
+      <c r="B45" s="14" t="s">
+        <v>222</v>
+      </c>
+      <c r="C45" s="18" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A46" s="13">
+        <v>298</v>
+      </c>
+      <c r="B46" s="14" t="s">
+        <v>223</v>
+      </c>
+      <c r="C46" s="18" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A47" s="13">
+        <v>299</v>
+      </c>
+      <c r="B47" s="14" t="s">
+        <v>224</v>
+      </c>
+      <c r="C47" s="18" t="s">
+        <v>130</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1868E1ED-CAEF-4CF4-8725-DD393E3F7908}">
+  <dimension ref="A1:C41"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A1" s="10" t="s">
+        <v>167</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>182</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A2" s="13">
+        <v>25</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>184</v>
+      </c>
+      <c r="C2" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A3" s="13">
+        <v>78</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>185</v>
+      </c>
+      <c r="C3" s="15">
+        <v>0.22000009640349694</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A4" s="13">
+        <v>79</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>186</v>
+      </c>
+      <c r="C4" s="15">
+        <v>0.22000000233362949</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A5" s="13">
+        <v>83</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>187</v>
+      </c>
+      <c r="C5" s="15">
+        <v>0.21999999999999997</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A6" s="13">
+        <v>84</v>
+      </c>
+      <c r="B6" s="14" t="s">
+        <v>188</v>
+      </c>
+      <c r="C6" s="15">
+        <v>0.21999189882532955</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A7" s="13">
+        <v>89</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>189</v>
+      </c>
+      <c r="C7" s="15">
+        <v>0.21983125793534719</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A8" s="13">
+        <v>92</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>190</v>
+      </c>
+      <c r="C8" s="15">
+        <v>0.22000005397585487</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A9" s="13">
+        <v>93</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="C9" s="15" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A10" s="13">
+        <v>98</v>
+      </c>
+      <c r="B10" s="14" t="s">
+        <v>193</v>
+      </c>
+      <c r="C10" s="15">
+        <v>0.21999999999999997</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A11" s="13">
+        <v>99</v>
+      </c>
+      <c r="B11" s="14" t="s">
+        <v>194</v>
+      </c>
+      <c r="C11" s="15">
+        <v>0.22000031853437774</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A12" s="13">
+        <v>102</v>
+      </c>
+      <c r="B12" s="14" t="s">
+        <v>195</v>
+      </c>
+      <c r="C12" s="15">
+        <v>0.22000007862284221</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A13" s="13">
+        <v>104</v>
+      </c>
+      <c r="B13" s="14" t="s">
+        <v>196</v>
+      </c>
+      <c r="C13" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A14" s="13">
+        <v>105</v>
+      </c>
+      <c r="B14" s="14" t="s">
+        <v>197</v>
+      </c>
+      <c r="C14" s="15">
+        <v>0.21999998775740814</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A15" s="13">
+        <v>118</v>
+      </c>
+      <c r="B15" s="14" t="s">
+        <v>198</v>
+      </c>
+      <c r="C15" s="15">
+        <v>0.22000002495421644</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A16" s="13">
+        <v>122</v>
+      </c>
+      <c r="B16" s="14" t="s">
+        <v>199</v>
+      </c>
+      <c r="C16" s="15">
+        <v>0.21999996233635133</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A17" s="13">
+        <v>139</v>
+      </c>
+      <c r="B17" s="14" t="s">
+        <v>200</v>
+      </c>
+      <c r="C17" s="15">
+        <v>0.21999999999999997</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A18" s="13">
+        <v>141</v>
+      </c>
+      <c r="B18" s="14" t="s">
+        <v>201</v>
+      </c>
+      <c r="C18" s="15">
+        <v>0.22000000791788321</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A19" s="13">
+        <v>145</v>
+      </c>
+      <c r="B19" s="14" t="s">
+        <v>202</v>
+      </c>
+      <c r="C19" s="15">
+        <v>0.21999999999999997</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A20" s="13">
+        <v>146</v>
+      </c>
+      <c r="B20" s="14" t="s">
+        <v>203</v>
+      </c>
+      <c r="C20" s="15">
+        <v>0.22000014950084057</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A21" s="13">
+        <v>147</v>
+      </c>
+      <c r="B21" s="14" t="s">
+        <v>204</v>
+      </c>
+      <c r="C21" s="15">
+        <v>0.21999997759842715</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A22" s="13">
+        <v>150</v>
+      </c>
+      <c r="B22" s="14" t="s">
+        <v>205</v>
+      </c>
+      <c r="C22" s="15">
+        <v>0.22000017095110525</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A23" s="13">
+        <v>160</v>
+      </c>
+      <c r="B23" s="14" t="s">
+        <v>206</v>
+      </c>
+      <c r="C23" s="15">
+        <v>0.22000005884402474</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A24" s="13">
+        <v>164</v>
+      </c>
+      <c r="B24" s="14" t="s">
+        <v>207</v>
+      </c>
+      <c r="C24" s="15">
+        <v>0.21712438709677429</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A25" s="13">
+        <v>178</v>
+      </c>
+      <c r="B25" s="14" t="s">
+        <v>208</v>
+      </c>
+      <c r="C25" s="15">
+        <v>1.8906838075475774E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A26" s="13">
+        <v>182</v>
+      </c>
+      <c r="B26" s="14" t="s">
+        <v>209</v>
+      </c>
+      <c r="C26" s="15">
+        <v>0.22000004861815081</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A27" s="13">
+        <v>210</v>
+      </c>
+      <c r="B27" s="14" t="s">
+        <v>210</v>
+      </c>
+      <c r="C27" s="15">
+        <v>0.21999992342585073</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A28" s="13">
+        <v>220</v>
+      </c>
+      <c r="B28" s="14" t="s">
+        <v>211</v>
+      </c>
+      <c r="C28" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A29" s="13">
+        <v>228</v>
+      </c>
+      <c r="B29" s="14" t="s">
+        <v>212</v>
+      </c>
+      <c r="C29" s="15">
+        <v>0.2200001696676368</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A30" s="13">
+        <v>235</v>
+      </c>
+      <c r="B30" s="14" t="s">
+        <v>213</v>
+      </c>
+      <c r="C30" s="15">
+        <v>0.21999999999999997</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A31" s="13">
+        <v>245</v>
+      </c>
+      <c r="B31" s="14" t="s">
+        <v>214</v>
+      </c>
+      <c r="C31" s="15">
+        <v>0.21999999188952324</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A32" s="13">
+        <v>250</v>
+      </c>
+      <c r="B32" s="14" t="s">
+        <v>215</v>
+      </c>
+      <c r="C32" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A33" s="13">
+        <v>256</v>
+      </c>
+      <c r="B33" s="14" t="s">
+        <v>216</v>
+      </c>
+      <c r="C33" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A34" s="13">
+        <v>263</v>
+      </c>
+      <c r="B34" s="14" t="s">
+        <v>217</v>
+      </c>
+      <c r="C34" s="15">
+        <v>0.22000004886685165</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A35" s="13">
+        <v>272</v>
+      </c>
+      <c r="B35" s="14" t="s">
+        <v>218</v>
+      </c>
+      <c r="C35" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A36" s="13">
+        <v>278</v>
+      </c>
+      <c r="B36" s="14" t="s">
+        <v>219</v>
+      </c>
+      <c r="C36" s="15">
+        <v>0.21999994762652597</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A37" s="13">
+        <v>290</v>
+      </c>
+      <c r="B37" s="14" t="s">
+        <v>220</v>
+      </c>
+      <c r="C37" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A38" s="13">
+        <v>291</v>
+      </c>
+      <c r="B38" s="14" t="s">
+        <v>221</v>
+      </c>
+      <c r="C38" s="15">
+        <v>0.22000156966182272</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A39" s="13">
+        <v>292</v>
+      </c>
+      <c r="B39" s="14" t="s">
+        <v>222</v>
+      </c>
+      <c r="C39" s="15">
+        <v>0.2200391544080269</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A40" s="13">
+        <v>298</v>
+      </c>
+      <c r="B40" s="14" t="s">
+        <v>223</v>
+      </c>
+      <c r="C40" s="15">
+        <v>0.22000004256548644</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A41" s="13">
+        <v>299</v>
+      </c>
+      <c r="B41" s="14" t="s">
+        <v>224</v>
+      </c>
+      <c r="C41" s="15">
+        <v>0.21999998523807074</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{375279E5-FD55-40B2-B98C-1A0E508B0195}">
+  <dimension ref="A1:B29"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A1" s="16" t="s">
+        <v>167</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A2" s="17">
+        <v>1891</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A3" s="17">
+        <v>1825</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A4" s="17">
+        <v>488</v>
+      </c>
+      <c r="B4" s="17" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A5" s="17">
+        <v>763</v>
+      </c>
+      <c r="B5" s="17" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A6" s="17">
+        <v>292</v>
+      </c>
+      <c r="B6" s="17" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A7" s="17">
+        <v>272</v>
+      </c>
+      <c r="B7" s="17" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A8" s="17">
+        <v>990</v>
+      </c>
+      <c r="B8" s="17" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A9" s="17">
+        <v>2656</v>
+      </c>
+      <c r="B9" s="17" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A10" s="17">
+        <v>2030</v>
+      </c>
+      <c r="B10" s="17" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A11" s="17">
+        <v>2082</v>
+      </c>
+      <c r="B11" s="17" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A12" s="17">
+        <v>841</v>
+      </c>
+      <c r="B12" s="17" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A13" s="17">
+        <v>250</v>
+      </c>
+      <c r="B13" s="17" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A14" s="17">
+        <v>385</v>
+      </c>
+      <c r="B14" s="17" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A15" s="17">
+        <v>381</v>
+      </c>
+      <c r="B15" s="17" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A16" s="17">
+        <v>444</v>
+      </c>
+      <c r="B16" s="17" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A17" s="17">
+        <v>2054</v>
+      </c>
+      <c r="B17" s="17" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A18" s="17">
+        <v>543</v>
+      </c>
+      <c r="B18" s="17" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A19" s="17">
+        <v>104</v>
+      </c>
+      <c r="B19" s="17" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A20" s="17">
+        <v>316</v>
+      </c>
+      <c r="B20" s="17" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A21" s="17">
+        <v>220</v>
+      </c>
+      <c r="B21" s="17" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A22" s="17">
+        <v>2079</v>
+      </c>
+      <c r="B22" s="17" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A23" s="17">
+        <v>290</v>
+      </c>
+      <c r="B23" s="17" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A24" s="17">
+        <v>634</v>
+      </c>
+      <c r="B24" s="17" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A25" s="17">
+        <v>1406</v>
+      </c>
+      <c r="B25" s="17" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A26" s="17">
+        <v>178</v>
+      </c>
+      <c r="B26" s="17" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A27" s="17">
+        <v>256</v>
+      </c>
+      <c r="B27" s="17" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A28" s="17">
+        <v>712</v>
+      </c>
+      <c r="B28" s="17" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A29" s="17">
+        <v>782</v>
+      </c>
+      <c r="B29" s="17" t="s">
+        <v>245</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1108AB1-127A-4D50-9F30-C7486AA9E608}">
+  <dimension ref="A1:C11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="3" max="3" width="17.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A1" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A2">
+        <v>178</v>
+      </c>
+      <c r="B2" t="s">
+        <v>170</v>
+      </c>
+      <c r="C2" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A3">
+        <v>634</v>
+      </c>
+      <c r="B3" t="s">
+        <v>172</v>
+      </c>
+      <c r="C3" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A4">
+        <v>1801</v>
+      </c>
+      <c r="B4" t="s">
+        <v>173</v>
+      </c>
+      <c r="C4" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A5">
+        <v>485</v>
+      </c>
+      <c r="B5" t="s">
+        <v>174</v>
+      </c>
+      <c r="C5" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A6">
+        <v>299</v>
+      </c>
+      <c r="B6" t="s">
+        <v>175</v>
+      </c>
+      <c r="C6" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A7">
+        <v>811</v>
+      </c>
+      <c r="B7" t="s">
+        <v>176</v>
+      </c>
+      <c r="C7" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A8">
+        <v>1825</v>
+      </c>
+      <c r="B8" t="s">
+        <v>177</v>
+      </c>
+      <c r="C8" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A9">
+        <v>1667</v>
+      </c>
+      <c r="B9" t="s">
+        <v>178</v>
+      </c>
+      <c r="C9" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A10">
+        <v>1408</v>
+      </c>
+      <c r="B10" t="s">
+        <v>180</v>
+      </c>
+      <c r="C10" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A11">
+        <v>1000</v>
+      </c>
+      <c r="B11" t="s">
+        <v>181</v>
+      </c>
+      <c r="C11" t="s">
+        <v>171</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F3E4911-66FD-46BA-85EE-7208A8CAC824}">
   <dimension ref="A1:F108"/>
   <sheetViews>
@@ -3240,7 +5078,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7659E2FF-6AAA-404D-9A14-3CE694ABA3A7}">
   <dimension ref="A1:C23"/>
   <sheetViews>
@@ -3511,11 +5349,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23F44718-4559-4977-A93C-2BC0306EBE28}">
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
@@ -3637,7 +5475,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F167614-BCFB-498C-B0A9-B06E506BC3D3}">
   <dimension ref="A1:B39"/>
   <sheetViews>

</xml_diff>

<commit_message>
AA - adjustments to file support_trascodifiche
</commit_message>
<xml_diff>
--- a/inputs/support_trascodifiche.xlsx
+++ b/inputs/support_trascodifiche.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://innovationteam-my.sharepoint.com/personal/a_abraham_innovationteam_eu/Documents/Documenti/progetti/22p11_Tool_FA/inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="21" documentId="8_{8C9F2755-18BA-4CE9-90D7-E32768AE5E81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{46DABB9F-EBF8-4667-8EA8-068A47AE97FE}"/>
+  <xr:revisionPtr revIDLastSave="24" documentId="8_{8C9F2755-18BA-4CE9-90D7-E32768AE5E81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8F60156C-6FFE-4444-AFBB-831A9BB6F3D9}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15675" xr2:uid="{9758A490-5BBA-4DAE-A128-35FF12EB83CB}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15675" activeTab="1" xr2:uid="{9758A490-5BBA-4DAE-A128-35FF12EB83CB}"/>
   </bookViews>
   <sheets>
     <sheet name="Condizioni_Commerciali" sheetId="7" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="806" uniqueCount="254">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="805" uniqueCount="253">
   <si>
     <t>$CON: Codice e descrizione</t>
   </si>
@@ -631,9 +631,6 @@
     <t>FRIULVINI SOCIETA'COOPERATIVA AGRIC</t>
   </si>
   <si>
-    <t>22,0%</t>
-  </si>
-  <si>
     <t>FURLANINA  SNC               *</t>
   </si>
   <si>
@@ -832,9 +829,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="0.0%"/>
-  </numFmts>
   <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1009,12 +1003,12 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="10" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -1022,33 +1016,6 @@
     <cellStyle name="Normale 7" xfId="2" xr:uid="{53EBC274-2193-4F8D-84F3-098F077B8327}"/>
   </cellStyles>
   <dxfs count="15">
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="0"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -1308,6 +1275,33 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1322,10 +1316,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{A4B5F73C-8C81-4BA0-9486-D78D8D2EDA32}" name="Elenco_Esportatori" displayName="Elenco_Esportatori" ref="A1:B29" totalsRowShown="0" headerRowDxfId="1" headerRowCellStyle="Normale 7" dataCellStyle="Normale 7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{A4B5F73C-8C81-4BA0-9486-D78D8D2EDA32}" name="Elenco_Esportatori" displayName="Elenco_Esportatori" ref="A1:B29" totalsRowShown="0" headerRowDxfId="14" headerRowCellStyle="Normale 7" dataCellStyle="Normale 7">
   <autoFilter ref="A1:B29" xr:uid="{A4B5F73C-8C81-4BA0-9486-D78D8D2EDA32}"/>
   <tableColumns count="2">
-    <tableColumn id="3" xr3:uid="{B1F89080-23D9-46D2-A0A2-ECC915269C09}" name="Soggetto" dataDxfId="0" dataCellStyle="Normale 7"/>
+    <tableColumn id="3" xr3:uid="{B1F89080-23D9-46D2-A0A2-ECC915269C09}" name="Soggetto" dataDxfId="13" dataCellStyle="Normale 7"/>
     <tableColumn id="2" xr3:uid="{6CE5CCEB-2876-4548-B4E6-7A22BC4AC5CA}" name="Ter_descr" dataCellStyle="Normale 7"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1333,10 +1327,10 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{A4CD4984-42E8-4E8F-9C29-4F867B1919A0}" name="Top_Clienti" displayName="Top_Clienti" ref="A1:C11" totalsRowShown="0" headerRowDxfId="14">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{A4CD4984-42E8-4E8F-9C29-4F867B1919A0}" name="Top_Clienti" displayName="Top_Clienti" ref="A1:C11" totalsRowShown="0" headerRowDxfId="12">
   <autoFilter ref="A1:C11" xr:uid="{A4CD4984-42E8-4E8F-9C29-4F867B1919A0}"/>
   <tableColumns count="3">
-    <tableColumn id="4" xr3:uid="{6AAC45EB-A00C-459D-8C5B-AC959ABE7DCD}" name="Soggetto" dataDxfId="13"/>
+    <tableColumn id="4" xr3:uid="{6AAC45EB-A00C-459D-8C5B-AC959ABE7DCD}" name="Soggetto" dataDxfId="11"/>
     <tableColumn id="2" xr3:uid="{7B6BFE59-FA92-466B-995F-DD6BD01640AB}" name="Descrizione"/>
     <tableColumn id="3" xr3:uid="{2088016D-F766-4701-8F36-DF5294CD2639}" name="Tipo cliente"/>
   </tableColumns>
@@ -1345,16 +1339,16 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{E832CCEC-F5F5-42D8-8383-1933DC5C8C1D}" name="Trascodifica_Analitico_CE" displayName="Trascodifica_Analitico_CE" ref="A1:F108" totalsRowShown="0" headerRowDxfId="12">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{E832CCEC-F5F5-42D8-8383-1933DC5C8C1D}" name="Trascodifica_Analitico_CE" displayName="Trascodifica_Analitico_CE" ref="A1:F108" totalsRowShown="0" headerRowDxfId="10">
   <autoFilter ref="A1:F108" xr:uid="{E832CCEC-F5F5-42D8-8383-1933DC5C8C1D}"/>
   <tableColumns count="6">
-    <tableColumn id="3" xr3:uid="{EDD3DE90-20FA-4C95-8697-6D0CFBD3D34A}" name="Chiave trascodifica" dataDxfId="11">
+    <tableColumn id="3" xr3:uid="{EDD3DE90-20FA-4C95-8697-6D0CFBD3D34A}" name="Chiave trascodifica" dataDxfId="9">
       <calculatedColumnFormula>+B2&amp;C2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="1" xr3:uid="{DB9DB5AC-9FF8-4926-8033-21AB8F0B4EFD}" name="$CDC: RAGGRUPPAMENTI_adj" dataDxfId="10"/>
+    <tableColumn id="1" xr3:uid="{DB9DB5AC-9FF8-4926-8033-21AB8F0B4EFD}" name="$CDC: RAGGRUPPAMENTI_adj" dataDxfId="8"/>
     <tableColumn id="2" xr3:uid="{06FBF0B0-A15D-4AFB-B465-7242820CF73D}" name="$CON: UNLG - Liv. 2"/>
-    <tableColumn id="4" xr3:uid="{794FE058-6F00-44B3-9FCF-51AA95F79206}" name="Trascodifica" dataDxfId="9"/>
-    <tableColumn id="5" xr3:uid="{DE8BD87C-828E-4931-A2F6-80DEA4839364}" name="Tipo voce" dataDxfId="8"/>
+    <tableColumn id="4" xr3:uid="{794FE058-6F00-44B3-9FCF-51AA95F79206}" name="Trascodifica" dataDxfId="7"/>
+    <tableColumn id="5" xr3:uid="{DE8BD87C-828E-4931-A2F6-80DEA4839364}" name="Tipo voce" dataDxfId="6"/>
     <tableColumn id="6" xr3:uid="{D7A74A4A-9FFA-42A1-A081-4618874B9909}" name="Note"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1362,19 +1356,19 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{18C42134-E9F8-4487-A759-0E0A55C87CC7}" name="Trascodifica_Condizioni_Commerciali" displayName="Trascodifica_Condizioni_Commerciali" ref="A1:C23" totalsRowShown="0" headerRowDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{18C42134-E9F8-4487-A759-0E0A55C87CC7}" name="Trascodifica_Condizioni_Commerciali" displayName="Trascodifica_Condizioni_Commerciali" ref="A1:C23" totalsRowShown="0" headerRowDxfId="5">
   <autoFilter ref="A1:C23" xr:uid="{18C42134-E9F8-4487-A759-0E0A55C87CC7}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{EEC8624E-B158-4B11-8B15-87315EDB7A65}" name="Condizioni commerciali nominali"/>
-    <tableColumn id="2" xr3:uid="{0E26CAB4-E054-46FC-9425-1C33322A5A5F}" name="Condizioni commerciali nominali_riclassificato" dataDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{F50EB424-39EE-40F9-9560-3D7FF968902F}" name="Modalità pagamento" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{0E26CAB4-E054-46FC-9425-1C33322A5A5F}" name="Condizioni commerciali nominali_riclassificato" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{F50EB424-39EE-40F9-9560-3D7FF968902F}" name="Modalità pagamento" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{3A8FC088-1845-4A45-A33F-B35A68332615}" name="Trascodifica_CdC" displayName="Trascodifica_CdC" ref="A1:B13" totalsRowShown="0" headerRowDxfId="4" headerRowCellStyle="Normale 2" dataCellStyle="Normale 2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{3A8FC088-1845-4A45-A33F-B35A68332615}" name="Trascodifica_CdC" displayName="Trascodifica_CdC" ref="A1:B13" totalsRowShown="0" headerRowDxfId="2" headerRowCellStyle="Normale 2" dataCellStyle="Normale 2">
   <autoFilter ref="A1:B13" xr:uid="{3A8FC088-1845-4A45-A33F-B35A68332615}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{7EA54190-3906-4667-AA7A-4FC8279040CA}" name="$CDC: RAGGRUPPAMENTI " dataCellStyle="Normale 2"/>
@@ -1385,11 +1379,11 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{42411417-7B51-4A46-A8D2-79D3CB8FE77A}" name="Trascodifica_Costo_Personale" displayName="Trascodifica_Costo_Personale" ref="A1:B39" totalsRowShown="0" headerRowDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{42411417-7B51-4A46-A8D2-79D3CB8FE77A}" name="Trascodifica_Costo_Personale" displayName="Trascodifica_Costo_Personale" ref="A1:B39" totalsRowShown="0" headerRowDxfId="1">
   <autoFilter ref="A1:B39" xr:uid="{42411417-7B51-4A46-A8D2-79D3CB8FE77A}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{41908B3F-CDCD-4896-B2C7-8E40BD4D38AA}" name="$CON: Codice e descrizione"/>
-    <tableColumn id="2" xr3:uid="{1BD768D9-BD65-4B3D-B940-62522AAB9168}" name="Tipo costo" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{1BD768D9-BD65-4B3D-B940-62522AAB9168}" name="Tipo costo" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1694,7 +1688,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8A799A3-2DEF-4D6D-A2E7-3FD643717F06}">
   <dimension ref="A1:C47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
@@ -1713,7 +1707,7 @@
         <v>182</v>
       </c>
       <c r="C1" s="12" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.45">
@@ -1721,9 +1715,9 @@
         <v>17</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>247</v>
-      </c>
-      <c r="C2" s="18" t="s">
+        <v>246</v>
+      </c>
+      <c r="C2" s="17" t="s">
         <v>135</v>
       </c>
     </row>
@@ -1734,7 +1728,7 @@
       <c r="B3" s="14" t="s">
         <v>184</v>
       </c>
-      <c r="C3" s="18" t="s">
+      <c r="C3" s="17" t="s">
         <v>124</v>
       </c>
     </row>
@@ -1743,9 +1737,9 @@
         <v>40</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>248</v>
-      </c>
-      <c r="C4" s="18" t="s">
+        <v>247</v>
+      </c>
+      <c r="C4" s="17" t="s">
         <v>135</v>
       </c>
     </row>
@@ -1756,7 +1750,7 @@
       <c r="B5" s="14" t="s">
         <v>185</v>
       </c>
-      <c r="C5" s="18" t="s">
+      <c r="C5" s="17" t="s">
         <v>141</v>
       </c>
     </row>
@@ -1767,7 +1761,7 @@
       <c r="B6" s="14" t="s">
         <v>186</v>
       </c>
-      <c r="C6" s="18" t="s">
+      <c r="C6" s="17" t="s">
         <v>127</v>
       </c>
     </row>
@@ -1776,9 +1770,9 @@
         <v>81</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>249</v>
-      </c>
-      <c r="C7" s="18" t="s">
+        <v>248</v>
+      </c>
+      <c r="C7" s="17" t="s">
         <v>124</v>
       </c>
     </row>
@@ -1789,7 +1783,7 @@
       <c r="B8" s="14" t="s">
         <v>187</v>
       </c>
-      <c r="C8" s="18" t="s">
+      <c r="C8" s="17" t="s">
         <v>127</v>
       </c>
     </row>
@@ -1800,7 +1794,7 @@
       <c r="B9" s="14" t="s">
         <v>188</v>
       </c>
-      <c r="C9" s="18" t="s">
+      <c r="C9" s="17" t="s">
         <v>130</v>
       </c>
     </row>
@@ -1811,7 +1805,7 @@
       <c r="B10" s="14" t="s">
         <v>189</v>
       </c>
-      <c r="C10" s="18" t="s">
+      <c r="C10" s="17" t="s">
         <v>127</v>
       </c>
     </row>
@@ -1822,7 +1816,7 @@
       <c r="B11" s="14" t="s">
         <v>190</v>
       </c>
-      <c r="C11" s="18" t="s">
+      <c r="C11" s="17" t="s">
         <v>127</v>
       </c>
     </row>
@@ -1833,7 +1827,7 @@
       <c r="B12" s="14" t="s">
         <v>191</v>
       </c>
-      <c r="C12" s="18" t="s">
+      <c r="C12" s="17" t="s">
         <v>127</v>
       </c>
     </row>
@@ -1842,9 +1836,9 @@
         <v>95</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>250</v>
-      </c>
-      <c r="C13" s="18" t="s">
+        <v>249</v>
+      </c>
+      <c r="C13" s="17" t="s">
         <v>124</v>
       </c>
     </row>
@@ -1853,9 +1847,9 @@
         <v>98</v>
       </c>
       <c r="B14" s="14" t="s">
-        <v>193</v>
-      </c>
-      <c r="C14" s="18" t="s">
+        <v>192</v>
+      </c>
+      <c r="C14" s="17" t="s">
         <v>127</v>
       </c>
     </row>
@@ -1864,9 +1858,9 @@
         <v>99</v>
       </c>
       <c r="B15" s="14" t="s">
-        <v>194</v>
-      </c>
-      <c r="C15" s="18" t="s">
+        <v>193</v>
+      </c>
+      <c r="C15" s="17" t="s">
         <v>124</v>
       </c>
     </row>
@@ -1875,9 +1869,9 @@
         <v>102</v>
       </c>
       <c r="B16" s="14" t="s">
-        <v>195</v>
-      </c>
-      <c r="C16" s="18" t="s">
+        <v>194</v>
+      </c>
+      <c r="C16" s="17" t="s">
         <v>124</v>
       </c>
     </row>
@@ -1886,9 +1880,9 @@
         <v>104</v>
       </c>
       <c r="B17" s="14" t="s">
-        <v>196</v>
-      </c>
-      <c r="C17" s="18" t="s">
+        <v>195</v>
+      </c>
+      <c r="C17" s="17" t="s">
         <v>127</v>
       </c>
     </row>
@@ -1897,9 +1891,9 @@
         <v>105</v>
       </c>
       <c r="B18" s="14" t="s">
-        <v>197</v>
-      </c>
-      <c r="C18" s="18" t="s">
+        <v>196</v>
+      </c>
+      <c r="C18" s="17" t="s">
         <v>124</v>
       </c>
     </row>
@@ -1908,9 +1902,9 @@
         <v>118</v>
       </c>
       <c r="B19" s="14" t="s">
-        <v>198</v>
-      </c>
-      <c r="C19" s="18" t="s">
+        <v>197</v>
+      </c>
+      <c r="C19" s="17" t="s">
         <v>124</v>
       </c>
     </row>
@@ -1919,10 +1913,10 @@
         <v>121</v>
       </c>
       <c r="B20" s="14" t="s">
+        <v>250</v>
+      </c>
+      <c r="C20" s="17" t="s">
         <v>251</v>
-      </c>
-      <c r="C20" s="18" t="s">
-        <v>252</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.45">
@@ -1930,9 +1924,9 @@
         <v>122</v>
       </c>
       <c r="B21" s="14" t="s">
-        <v>199</v>
-      </c>
-      <c r="C21" s="18" t="s">
+        <v>198</v>
+      </c>
+      <c r="C21" s="17" t="s">
         <v>131</v>
       </c>
     </row>
@@ -1941,9 +1935,9 @@
         <v>128</v>
       </c>
       <c r="B22" s="14" t="s">
-        <v>253</v>
-      </c>
-      <c r="C22" s="18" t="s">
+        <v>252</v>
+      </c>
+      <c r="C22" s="17" t="s">
         <v>130</v>
       </c>
     </row>
@@ -1952,9 +1946,9 @@
         <v>139</v>
       </c>
       <c r="B23" s="14" t="s">
-        <v>200</v>
-      </c>
-      <c r="C23" s="18" t="s">
+        <v>199</v>
+      </c>
+      <c r="C23" s="17" t="s">
         <v>130</v>
       </c>
     </row>
@@ -1963,9 +1957,9 @@
         <v>141</v>
       </c>
       <c r="B24" s="14" t="s">
-        <v>201</v>
-      </c>
-      <c r="C24" s="18" t="s">
+        <v>200</v>
+      </c>
+      <c r="C24" s="17" t="s">
         <v>127</v>
       </c>
     </row>
@@ -1974,9 +1968,9 @@
         <v>145</v>
       </c>
       <c r="B25" s="14" t="s">
-        <v>202</v>
-      </c>
-      <c r="C25" s="18" t="s">
+        <v>201</v>
+      </c>
+      <c r="C25" s="17" t="s">
         <v>124</v>
       </c>
     </row>
@@ -1985,9 +1979,9 @@
         <v>146</v>
       </c>
       <c r="B26" s="14" t="s">
-        <v>203</v>
-      </c>
-      <c r="C26" s="18" t="s">
+        <v>202</v>
+      </c>
+      <c r="C26" s="17" t="s">
         <v>133</v>
       </c>
     </row>
@@ -1996,9 +1990,9 @@
         <v>147</v>
       </c>
       <c r="B27" s="14" t="s">
-        <v>204</v>
-      </c>
-      <c r="C27" s="18" t="s">
+        <v>203</v>
+      </c>
+      <c r="C27" s="17" t="s">
         <v>124</v>
       </c>
     </row>
@@ -2007,9 +2001,9 @@
         <v>150</v>
       </c>
       <c r="B28" s="14" t="s">
-        <v>205</v>
-      </c>
-      <c r="C28" s="18" t="s">
+        <v>204</v>
+      </c>
+      <c r="C28" s="17" t="s">
         <v>139</v>
       </c>
     </row>
@@ -2018,9 +2012,9 @@
         <v>160</v>
       </c>
       <c r="B29" s="14" t="s">
-        <v>206</v>
-      </c>
-      <c r="C29" s="18" t="s">
+        <v>205</v>
+      </c>
+      <c r="C29" s="17" t="s">
         <v>127</v>
       </c>
     </row>
@@ -2029,9 +2023,9 @@
         <v>164</v>
       </c>
       <c r="B30" s="14" t="s">
-        <v>207</v>
-      </c>
-      <c r="C30" s="18" t="s">
+        <v>206</v>
+      </c>
+      <c r="C30" s="17" t="s">
         <v>127</v>
       </c>
     </row>
@@ -2040,9 +2034,9 @@
         <v>178</v>
       </c>
       <c r="B31" s="14" t="s">
-        <v>208</v>
-      </c>
-      <c r="C31" s="18" t="s">
+        <v>207</v>
+      </c>
+      <c r="C31" s="17" t="s">
         <v>124</v>
       </c>
     </row>
@@ -2051,9 +2045,9 @@
         <v>182</v>
       </c>
       <c r="B32" s="14" t="s">
-        <v>209</v>
-      </c>
-      <c r="C32" s="18" t="s">
+        <v>208</v>
+      </c>
+      <c r="C32" s="17" t="s">
         <v>124</v>
       </c>
     </row>
@@ -2062,9 +2056,9 @@
         <v>210</v>
       </c>
       <c r="B33" s="14" t="s">
-        <v>210</v>
-      </c>
-      <c r="C33" s="18" t="s">
+        <v>209</v>
+      </c>
+      <c r="C33" s="17" t="s">
         <v>130</v>
       </c>
     </row>
@@ -2073,9 +2067,9 @@
         <v>220</v>
       </c>
       <c r="B34" s="14" t="s">
-        <v>211</v>
-      </c>
-      <c r="C34" s="18" t="s">
+        <v>210</v>
+      </c>
+      <c r="C34" s="17" t="s">
         <v>124</v>
       </c>
     </row>
@@ -2084,9 +2078,9 @@
         <v>228</v>
       </c>
       <c r="B35" s="14" t="s">
-        <v>212</v>
-      </c>
-      <c r="C35" s="18" t="s">
+        <v>211</v>
+      </c>
+      <c r="C35" s="17" t="s">
         <v>124</v>
       </c>
     </row>
@@ -2095,9 +2089,9 @@
         <v>235</v>
       </c>
       <c r="B36" s="14" t="s">
-        <v>213</v>
-      </c>
-      <c r="C36" s="18" t="s">
+        <v>212</v>
+      </c>
+      <c r="C36" s="17" t="s">
         <v>138</v>
       </c>
     </row>
@@ -2106,9 +2100,9 @@
         <v>245</v>
       </c>
       <c r="B37" s="14" t="s">
-        <v>214</v>
-      </c>
-      <c r="C37" s="18" t="s">
+        <v>213</v>
+      </c>
+      <c r="C37" s="17" t="s">
         <v>127</v>
       </c>
     </row>
@@ -2117,9 +2111,9 @@
         <v>250</v>
       </c>
       <c r="B38" s="14" t="s">
-        <v>215</v>
-      </c>
-      <c r="C38" s="18" t="s">
+        <v>214</v>
+      </c>
+      <c r="C38" s="17" t="s">
         <v>124</v>
       </c>
     </row>
@@ -2128,9 +2122,9 @@
         <v>256</v>
       </c>
       <c r="B39" s="14" t="s">
-        <v>216</v>
-      </c>
-      <c r="C39" s="18" t="s">
+        <v>215</v>
+      </c>
+      <c r="C39" s="17" t="s">
         <v>124</v>
       </c>
     </row>
@@ -2139,9 +2133,9 @@
         <v>263</v>
       </c>
       <c r="B40" s="14" t="s">
-        <v>217</v>
-      </c>
-      <c r="C40" s="18" t="s">
+        <v>216</v>
+      </c>
+      <c r="C40" s="17" t="s">
         <v>124</v>
       </c>
     </row>
@@ -2150,9 +2144,9 @@
         <v>272</v>
       </c>
       <c r="B41" s="14" t="s">
-        <v>218</v>
-      </c>
-      <c r="C41" s="18" t="s">
+        <v>217</v>
+      </c>
+      <c r="C41" s="17" t="s">
         <v>127</v>
       </c>
     </row>
@@ -2161,9 +2155,9 @@
         <v>278</v>
       </c>
       <c r="B42" s="14" t="s">
-        <v>219</v>
-      </c>
-      <c r="C42" s="18" t="s">
+        <v>218</v>
+      </c>
+      <c r="C42" s="17" t="s">
         <v>127</v>
       </c>
     </row>
@@ -2172,9 +2166,9 @@
         <v>290</v>
       </c>
       <c r="B43" s="14" t="s">
-        <v>220</v>
-      </c>
-      <c r="C43" s="18" t="s">
+        <v>219</v>
+      </c>
+      <c r="C43" s="17" t="s">
         <v>135</v>
       </c>
     </row>
@@ -2183,9 +2177,9 @@
         <v>291</v>
       </c>
       <c r="B44" s="14" t="s">
-        <v>221</v>
-      </c>
-      <c r="C44" s="18" t="s">
+        <v>220</v>
+      </c>
+      <c r="C44" s="17" t="s">
         <v>124</v>
       </c>
     </row>
@@ -2194,9 +2188,9 @@
         <v>292</v>
       </c>
       <c r="B45" s="14" t="s">
-        <v>222</v>
-      </c>
-      <c r="C45" s="18" t="s">
+        <v>221</v>
+      </c>
+      <c r="C45" s="17" t="s">
         <v>124</v>
       </c>
     </row>
@@ -2205,9 +2199,9 @@
         <v>298</v>
       </c>
       <c r="B46" s="14" t="s">
-        <v>223</v>
-      </c>
-      <c r="C46" s="18" t="s">
+        <v>222</v>
+      </c>
+      <c r="C46" s="17" t="s">
         <v>127</v>
       </c>
     </row>
@@ -2216,9 +2210,9 @@
         <v>299</v>
       </c>
       <c r="B47" s="14" t="s">
-        <v>224</v>
-      </c>
-      <c r="C47" s="18" t="s">
+        <v>223</v>
+      </c>
+      <c r="C47" s="17" t="s">
         <v>130</v>
       </c>
     </row>
@@ -2231,8 +2225,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1868E1ED-CAEF-4CF4-8725-DD393E3F7908}">
   <dimension ref="A1:C41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2255,7 +2249,7 @@
       <c r="B2" s="14" t="s">
         <v>184</v>
       </c>
-      <c r="C2" s="15">
+      <c r="C2" s="18">
         <v>0</v>
       </c>
     </row>
@@ -2266,7 +2260,7 @@
       <c r="B3" s="14" t="s">
         <v>185</v>
       </c>
-      <c r="C3" s="15">
+      <c r="C3" s="18">
         <v>0.22000009640349694</v>
       </c>
     </row>
@@ -2277,7 +2271,7 @@
       <c r="B4" s="14" t="s">
         <v>186</v>
       </c>
-      <c r="C4" s="15">
+      <c r="C4" s="18">
         <v>0.22000000233362949</v>
       </c>
     </row>
@@ -2288,7 +2282,7 @@
       <c r="B5" s="14" t="s">
         <v>187</v>
       </c>
-      <c r="C5" s="15">
+      <c r="C5" s="18">
         <v>0.21999999999999997</v>
       </c>
     </row>
@@ -2299,7 +2293,7 @@
       <c r="B6" s="14" t="s">
         <v>188</v>
       </c>
-      <c r="C6" s="15">
+      <c r="C6" s="18">
         <v>0.21999189882532955</v>
       </c>
     </row>
@@ -2310,7 +2304,7 @@
       <c r="B7" s="14" t="s">
         <v>189</v>
       </c>
-      <c r="C7" s="15">
+      <c r="C7" s="18">
         <v>0.21983125793534719</v>
       </c>
     </row>
@@ -2321,7 +2315,7 @@
       <c r="B8" s="14" t="s">
         <v>190</v>
       </c>
-      <c r="C8" s="15">
+      <c r="C8" s="18">
         <v>0.22000005397585487</v>
       </c>
     </row>
@@ -2332,8 +2326,8 @@
       <c r="B9" s="14" t="s">
         <v>191</v>
       </c>
-      <c r="C9" s="15" t="s">
-        <v>192</v>
+      <c r="C9" s="18">
+        <v>0.22</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.45">
@@ -2341,9 +2335,9 @@
         <v>98</v>
       </c>
       <c r="B10" s="14" t="s">
-        <v>193</v>
-      </c>
-      <c r="C10" s="15">
+        <v>192</v>
+      </c>
+      <c r="C10" s="18">
         <v>0.21999999999999997</v>
       </c>
     </row>
@@ -2352,9 +2346,9 @@
         <v>99</v>
       </c>
       <c r="B11" s="14" t="s">
-        <v>194</v>
-      </c>
-      <c r="C11" s="15">
+        <v>193</v>
+      </c>
+      <c r="C11" s="18">
         <v>0.22000031853437774</v>
       </c>
     </row>
@@ -2363,9 +2357,9 @@
         <v>102</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>195</v>
-      </c>
-      <c r="C12" s="15">
+        <v>194</v>
+      </c>
+      <c r="C12" s="18">
         <v>0.22000007862284221</v>
       </c>
     </row>
@@ -2374,9 +2368,9 @@
         <v>104</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>196</v>
-      </c>
-      <c r="C13" s="15">
+        <v>195</v>
+      </c>
+      <c r="C13" s="18">
         <v>0</v>
       </c>
     </row>
@@ -2385,9 +2379,9 @@
         <v>105</v>
       </c>
       <c r="B14" s="14" t="s">
-        <v>197</v>
-      </c>
-      <c r="C14" s="15">
+        <v>196</v>
+      </c>
+      <c r="C14" s="18">
         <v>0.21999998775740814</v>
       </c>
     </row>
@@ -2396,9 +2390,9 @@
         <v>118</v>
       </c>
       <c r="B15" s="14" t="s">
-        <v>198</v>
-      </c>
-      <c r="C15" s="15">
+        <v>197</v>
+      </c>
+      <c r="C15" s="18">
         <v>0.22000002495421644</v>
       </c>
     </row>
@@ -2407,9 +2401,9 @@
         <v>122</v>
       </c>
       <c r="B16" s="14" t="s">
-        <v>199</v>
-      </c>
-      <c r="C16" s="15">
+        <v>198</v>
+      </c>
+      <c r="C16" s="18">
         <v>0.21999996233635133</v>
       </c>
     </row>
@@ -2418,9 +2412,9 @@
         <v>139</v>
       </c>
       <c r="B17" s="14" t="s">
-        <v>200</v>
-      </c>
-      <c r="C17" s="15">
+        <v>199</v>
+      </c>
+      <c r="C17" s="18">
         <v>0.21999999999999997</v>
       </c>
     </row>
@@ -2429,9 +2423,9 @@
         <v>141</v>
       </c>
       <c r="B18" s="14" t="s">
-        <v>201</v>
-      </c>
-      <c r="C18" s="15">
+        <v>200</v>
+      </c>
+      <c r="C18" s="18">
         <v>0.22000000791788321</v>
       </c>
     </row>
@@ -2440,9 +2434,9 @@
         <v>145</v>
       </c>
       <c r="B19" s="14" t="s">
-        <v>202</v>
-      </c>
-      <c r="C19" s="15">
+        <v>201</v>
+      </c>
+      <c r="C19" s="18">
         <v>0.21999999999999997</v>
       </c>
     </row>
@@ -2451,9 +2445,9 @@
         <v>146</v>
       </c>
       <c r="B20" s="14" t="s">
-        <v>203</v>
-      </c>
-      <c r="C20" s="15">
+        <v>202</v>
+      </c>
+      <c r="C20" s="18">
         <v>0.22000014950084057</v>
       </c>
     </row>
@@ -2462,9 +2456,9 @@
         <v>147</v>
       </c>
       <c r="B21" s="14" t="s">
-        <v>204</v>
-      </c>
-      <c r="C21" s="15">
+        <v>203</v>
+      </c>
+      <c r="C21" s="18">
         <v>0.21999997759842715</v>
       </c>
     </row>
@@ -2473,9 +2467,9 @@
         <v>150</v>
       </c>
       <c r="B22" s="14" t="s">
-        <v>205</v>
-      </c>
-      <c r="C22" s="15">
+        <v>204</v>
+      </c>
+      <c r="C22" s="18">
         <v>0.22000017095110525</v>
       </c>
     </row>
@@ -2484,9 +2478,9 @@
         <v>160</v>
       </c>
       <c r="B23" s="14" t="s">
-        <v>206</v>
-      </c>
-      <c r="C23" s="15">
+        <v>205</v>
+      </c>
+      <c r="C23" s="18">
         <v>0.22000005884402474</v>
       </c>
     </row>
@@ -2495,9 +2489,9 @@
         <v>164</v>
       </c>
       <c r="B24" s="14" t="s">
-        <v>207</v>
-      </c>
-      <c r="C24" s="15">
+        <v>206</v>
+      </c>
+      <c r="C24" s="18">
         <v>0.21712438709677429</v>
       </c>
     </row>
@@ -2506,9 +2500,9 @@
         <v>178</v>
       </c>
       <c r="B25" s="14" t="s">
-        <v>208</v>
-      </c>
-      <c r="C25" s="15">
+        <v>207</v>
+      </c>
+      <c r="C25" s="18">
         <v>1.8906838075475774E-2</v>
       </c>
     </row>
@@ -2517,9 +2511,9 @@
         <v>182</v>
       </c>
       <c r="B26" s="14" t="s">
-        <v>209</v>
-      </c>
-      <c r="C26" s="15">
+        <v>208</v>
+      </c>
+      <c r="C26" s="18">
         <v>0.22000004861815081</v>
       </c>
     </row>
@@ -2528,9 +2522,9 @@
         <v>210</v>
       </c>
       <c r="B27" s="14" t="s">
-        <v>210</v>
-      </c>
-      <c r="C27" s="15">
+        <v>209</v>
+      </c>
+      <c r="C27" s="18">
         <v>0.21999992342585073</v>
       </c>
     </row>
@@ -2539,9 +2533,9 @@
         <v>220</v>
       </c>
       <c r="B28" s="14" t="s">
-        <v>211</v>
-      </c>
-      <c r="C28" s="15">
+        <v>210</v>
+      </c>
+      <c r="C28" s="18">
         <v>0</v>
       </c>
     </row>
@@ -2550,9 +2544,9 @@
         <v>228</v>
       </c>
       <c r="B29" s="14" t="s">
-        <v>212</v>
-      </c>
-      <c r="C29" s="15">
+        <v>211</v>
+      </c>
+      <c r="C29" s="18">
         <v>0.2200001696676368</v>
       </c>
     </row>
@@ -2561,9 +2555,9 @@
         <v>235</v>
       </c>
       <c r="B30" s="14" t="s">
-        <v>213</v>
-      </c>
-      <c r="C30" s="15">
+        <v>212</v>
+      </c>
+      <c r="C30" s="18">
         <v>0.21999999999999997</v>
       </c>
     </row>
@@ -2572,9 +2566,9 @@
         <v>245</v>
       </c>
       <c r="B31" s="14" t="s">
-        <v>214</v>
-      </c>
-      <c r="C31" s="15">
+        <v>213</v>
+      </c>
+      <c r="C31" s="18">
         <v>0.21999999188952324</v>
       </c>
     </row>
@@ -2583,9 +2577,9 @@
         <v>250</v>
       </c>
       <c r="B32" s="14" t="s">
-        <v>215</v>
-      </c>
-      <c r="C32" s="15">
+        <v>214</v>
+      </c>
+      <c r="C32" s="18">
         <v>0</v>
       </c>
     </row>
@@ -2594,9 +2588,9 @@
         <v>256</v>
       </c>
       <c r="B33" s="14" t="s">
-        <v>216</v>
-      </c>
-      <c r="C33" s="15">
+        <v>215</v>
+      </c>
+      <c r="C33" s="18">
         <v>0</v>
       </c>
     </row>
@@ -2605,9 +2599,9 @@
         <v>263</v>
       </c>
       <c r="B34" s="14" t="s">
-        <v>217</v>
-      </c>
-      <c r="C34" s="15">
+        <v>216</v>
+      </c>
+      <c r="C34" s="18">
         <v>0.22000004886685165</v>
       </c>
     </row>
@@ -2616,9 +2610,9 @@
         <v>272</v>
       </c>
       <c r="B35" s="14" t="s">
-        <v>218</v>
-      </c>
-      <c r="C35" s="15">
+        <v>217</v>
+      </c>
+      <c r="C35" s="18">
         <v>0</v>
       </c>
     </row>
@@ -2627,9 +2621,9 @@
         <v>278</v>
       </c>
       <c r="B36" s="14" t="s">
-        <v>219</v>
-      </c>
-      <c r="C36" s="15">
+        <v>218</v>
+      </c>
+      <c r="C36" s="18">
         <v>0.21999994762652597</v>
       </c>
     </row>
@@ -2638,9 +2632,9 @@
         <v>290</v>
       </c>
       <c r="B37" s="14" t="s">
-        <v>220</v>
-      </c>
-      <c r="C37" s="15">
+        <v>219</v>
+      </c>
+      <c r="C37" s="18">
         <v>0</v>
       </c>
     </row>
@@ -2649,9 +2643,9 @@
         <v>291</v>
       </c>
       <c r="B38" s="14" t="s">
-        <v>221</v>
-      </c>
-      <c r="C38" s="15">
+        <v>220</v>
+      </c>
+      <c r="C38" s="18">
         <v>0.22000156966182272</v>
       </c>
     </row>
@@ -2660,9 +2654,9 @@
         <v>292</v>
       </c>
       <c r="B39" s="14" t="s">
-        <v>222</v>
-      </c>
-      <c r="C39" s="15">
+        <v>221</v>
+      </c>
+      <c r="C39" s="18">
         <v>0.2200391544080269</v>
       </c>
     </row>
@@ -2671,9 +2665,9 @@
         <v>298</v>
       </c>
       <c r="B40" s="14" t="s">
-        <v>223</v>
-      </c>
-      <c r="C40" s="15">
+        <v>222</v>
+      </c>
+      <c r="C40" s="18">
         <v>0.22000004256548644</v>
       </c>
     </row>
@@ -2682,9 +2676,9 @@
         <v>299</v>
       </c>
       <c r="B41" s="14" t="s">
-        <v>224</v>
-      </c>
-      <c r="C41" s="15">
+        <v>223</v>
+      </c>
+      <c r="C41" s="18">
         <v>0.21999998523807074</v>
       </c>
     </row>
@@ -2704,235 +2698,235 @@
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="15" t="s">
         <v>167</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="15" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A2" s="16">
+        <v>1891</v>
+      </c>
+      <c r="B2" s="16" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A2" s="17">
-        <v>1891</v>
-      </c>
-      <c r="B2" s="17" t="s">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A3" s="16">
+        <v>1825</v>
+      </c>
+      <c r="B3" s="16" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A3" s="17">
-        <v>1825</v>
-      </c>
-      <c r="B3" s="17" t="s">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A4" s="16">
+        <v>488</v>
+      </c>
+      <c r="B4" s="16" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A4" s="17">
-        <v>488</v>
-      </c>
-      <c r="B4" s="17" t="s">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A5" s="16">
+        <v>763</v>
+      </c>
+      <c r="B5" s="16" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A5" s="17">
-        <v>763</v>
-      </c>
-      <c r="B5" s="17" t="s">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A6" s="16">
+        <v>292</v>
+      </c>
+      <c r="B6" s="16" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A7" s="16">
+        <v>272</v>
+      </c>
+      <c r="B7" s="16" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A8" s="16">
+        <v>990</v>
+      </c>
+      <c r="B8" s="16" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A6" s="17">
-        <v>292</v>
-      </c>
-      <c r="B6" s="17" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A7" s="17">
-        <v>272</v>
-      </c>
-      <c r="B7" s="17" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A8" s="17">
-        <v>990</v>
-      </c>
-      <c r="B8" s="17" t="s">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A9" s="16">
+        <v>2656</v>
+      </c>
+      <c r="B9" s="16" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A9" s="17">
-        <v>2656</v>
-      </c>
-      <c r="B9" s="17" t="s">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A10" s="16">
+        <v>2030</v>
+      </c>
+      <c r="B10" s="16" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A10" s="17">
-        <v>2030</v>
-      </c>
-      <c r="B10" s="17" t="s">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A11" s="16">
+        <v>2082</v>
+      </c>
+      <c r="B11" s="16" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A11" s="17">
-        <v>2082</v>
-      </c>
-      <c r="B11" s="17" t="s">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A12" s="16">
+        <v>841</v>
+      </c>
+      <c r="B12" s="16" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A12" s="17">
-        <v>841</v>
-      </c>
-      <c r="B12" s="17" t="s">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A13" s="16">
+        <v>250</v>
+      </c>
+      <c r="B13" s="16" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A14" s="16">
+        <v>385</v>
+      </c>
+      <c r="B14" s="16" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A13" s="17">
-        <v>250</v>
-      </c>
-      <c r="B13" s="17" t="s">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A15" s="16">
+        <v>381</v>
+      </c>
+      <c r="B15" s="16" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A16" s="16">
+        <v>444</v>
+      </c>
+      <c r="B16" s="16" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A17" s="16">
+        <v>2054</v>
+      </c>
+      <c r="B17" s="16" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A18" s="16">
+        <v>543</v>
+      </c>
+      <c r="B18" s="16" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A19" s="16">
+        <v>104</v>
+      </c>
+      <c r="B19" s="16" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A20" s="16">
+        <v>316</v>
+      </c>
+      <c r="B20" s="16" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A21" s="16">
+        <v>220</v>
+      </c>
+      <c r="B21" s="16" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A22" s="16">
+        <v>2079</v>
+      </c>
+      <c r="B22" s="16" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A23" s="16">
+        <v>290</v>
+      </c>
+      <c r="B23" s="16" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A24" s="16">
+        <v>634</v>
+      </c>
+      <c r="B24" s="16" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A25" s="16">
+        <v>1406</v>
+      </c>
+      <c r="B25" s="16" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A26" s="16">
+        <v>178</v>
+      </c>
+      <c r="B26" s="16" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A27" s="16">
+        <v>256</v>
+      </c>
+      <c r="B27" s="16" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A14" s="17">
-        <v>385</v>
-      </c>
-      <c r="B14" s="17" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A15" s="17">
-        <v>381</v>
-      </c>
-      <c r="B15" s="17" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A16" s="17">
-        <v>444</v>
-      </c>
-      <c r="B16" s="17" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A17" s="17">
-        <v>2054</v>
-      </c>
-      <c r="B17" s="17" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A18" s="17">
-        <v>543</v>
-      </c>
-      <c r="B18" s="17" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A19" s="17">
-        <v>104</v>
-      </c>
-      <c r="B19" s="17" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A20" s="17">
-        <v>316</v>
-      </c>
-      <c r="B20" s="17" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A21" s="17">
-        <v>220</v>
-      </c>
-      <c r="B21" s="17" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A22" s="17">
-        <v>2079</v>
-      </c>
-      <c r="B22" s="17" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A23" s="17">
-        <v>290</v>
-      </c>
-      <c r="B23" s="17" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A24" s="17">
-        <v>634</v>
-      </c>
-      <c r="B24" s="17" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A25" s="17">
-        <v>1406</v>
-      </c>
-      <c r="B25" s="17" t="s">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A28" s="16">
+        <v>712</v>
+      </c>
+      <c r="B28" s="16" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A26" s="17">
-        <v>178</v>
-      </c>
-      <c r="B26" s="17" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A27" s="17">
-        <v>256</v>
-      </c>
-      <c r="B27" s="17" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A28" s="17">
-        <v>712</v>
-      </c>
-      <c r="B28" s="17" t="s">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A29" s="16">
+        <v>782</v>
+      </c>
+      <c r="B29" s="16" t="s">
         <v>244</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A29" s="17">
-        <v>782</v>
-      </c>
-      <c r="B29" s="17" t="s">
-        <v>245</v>
       </c>
     </row>
   </sheetData>
@@ -5087,6 +5081,9 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="2" max="2" width="24.796875" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A1" s="6" t="s">

</xml_diff>

<commit_message>
Aggiunta foglio con top clienti
</commit_message>
<xml_diff>
--- a/inputs/support_trascodifiche.xlsx
+++ b/inputs/support_trascodifiche.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://innovationteam-my.sharepoint.com/personal/a_abraham_innovationteam_eu/Documents/Documenti/progetti/22p11_Tool_FA/inputs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LUP\Documents\GitHub\22p11_Tool_FA\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="24" documentId="8_{8C9F2755-18BA-4CE9-90D7-E32768AE5E81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8F60156C-6FFE-4444-AFBB-831A9BB6F3D9}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C924B778-F903-4A3B-9F82-7C4D2B65AC31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15675" activeTab="1" xr2:uid="{9758A490-5BBA-4DAE-A128-35FF12EB83CB}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" firstSheet="5" activeTab="8" xr2:uid="{9758A490-5BBA-4DAE-A128-35FF12EB83CB}"/>
   </bookViews>
   <sheets>
     <sheet name="Condizioni_Commerciali" sheetId="7" r:id="rId1"/>
@@ -21,6 +21,7 @@
     <sheet name="Trascodifica_Condizioni_comm_li" sheetId="3" r:id="rId6"/>
     <sheet name="Trascodifica_CdC" sheetId="4" r:id="rId7"/>
     <sheet name="Trascodifica_Costo_Personale" sheetId="1" r:id="rId8"/>
+    <sheet name="Top clienti" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="805" uniqueCount="253">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="828" uniqueCount="253">
   <si>
     <t>$CON: Codice e descrizione</t>
   </si>
@@ -1015,7 +1016,34 @@
     <cellStyle name="Normale 2" xfId="1" xr:uid="{3D0E86AB-4D3C-45D0-B0FD-4FA2CF8A5195}"/>
     <cellStyle name="Normale 7" xfId="2" xr:uid="{53EBC274-2193-4F8D-84F3-098F077B8327}"/>
   </cellStyles>
-  <dxfs count="15">
+  <dxfs count="17">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -1316,10 +1344,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{A4B5F73C-8C81-4BA0-9486-D78D8D2EDA32}" name="Elenco_Esportatori" displayName="Elenco_Esportatori" ref="A1:B29" totalsRowShown="0" headerRowDxfId="14" headerRowCellStyle="Normale 7" dataCellStyle="Normale 7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{A4B5F73C-8C81-4BA0-9486-D78D8D2EDA32}" name="Elenco_Esportatori" displayName="Elenco_Esportatori" ref="A1:B29" totalsRowShown="0" headerRowDxfId="16" headerRowCellStyle="Normale 7" dataCellStyle="Normale 7">
   <autoFilter ref="A1:B29" xr:uid="{A4B5F73C-8C81-4BA0-9486-D78D8D2EDA32}"/>
   <tableColumns count="2">
-    <tableColumn id="3" xr3:uid="{B1F89080-23D9-46D2-A0A2-ECC915269C09}" name="Soggetto" dataDxfId="13" dataCellStyle="Normale 7"/>
+    <tableColumn id="3" xr3:uid="{B1F89080-23D9-46D2-A0A2-ECC915269C09}" name="Soggetto" dataDxfId="15" dataCellStyle="Normale 7"/>
     <tableColumn id="2" xr3:uid="{6CE5CCEB-2876-4548-B4E6-7A22BC4AC5CA}" name="Ter_descr" dataCellStyle="Normale 7"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1327,10 +1355,10 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{A4CD4984-42E8-4E8F-9C29-4F867B1919A0}" name="Top_Clienti" displayName="Top_Clienti" ref="A1:C11" totalsRowShown="0" headerRowDxfId="12">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{A4CD4984-42E8-4E8F-9C29-4F867B1919A0}" name="Top_Clienti" displayName="Top_Clienti" ref="A1:C11" totalsRowShown="0" headerRowDxfId="14">
   <autoFilter ref="A1:C11" xr:uid="{A4CD4984-42E8-4E8F-9C29-4F867B1919A0}"/>
   <tableColumns count="3">
-    <tableColumn id="4" xr3:uid="{6AAC45EB-A00C-459D-8C5B-AC959ABE7DCD}" name="Soggetto" dataDxfId="11"/>
+    <tableColumn id="4" xr3:uid="{6AAC45EB-A00C-459D-8C5B-AC959ABE7DCD}" name="Soggetto" dataDxfId="13"/>
     <tableColumn id="2" xr3:uid="{7B6BFE59-FA92-466B-995F-DD6BD01640AB}" name="Descrizione"/>
     <tableColumn id="3" xr3:uid="{2088016D-F766-4701-8F36-DF5294CD2639}" name="Tipo cliente"/>
   </tableColumns>
@@ -1339,16 +1367,16 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{E832CCEC-F5F5-42D8-8383-1933DC5C8C1D}" name="Trascodifica_Analitico_CE" displayName="Trascodifica_Analitico_CE" ref="A1:F108" totalsRowShown="0" headerRowDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{E832CCEC-F5F5-42D8-8383-1933DC5C8C1D}" name="Trascodifica_Analitico_CE" displayName="Trascodifica_Analitico_CE" ref="A1:F108" totalsRowShown="0" headerRowDxfId="12">
   <autoFilter ref="A1:F108" xr:uid="{E832CCEC-F5F5-42D8-8383-1933DC5C8C1D}"/>
   <tableColumns count="6">
-    <tableColumn id="3" xr3:uid="{EDD3DE90-20FA-4C95-8697-6D0CFBD3D34A}" name="Chiave trascodifica" dataDxfId="9">
+    <tableColumn id="3" xr3:uid="{EDD3DE90-20FA-4C95-8697-6D0CFBD3D34A}" name="Chiave trascodifica" dataDxfId="11">
       <calculatedColumnFormula>+B2&amp;C2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="1" xr3:uid="{DB9DB5AC-9FF8-4926-8033-21AB8F0B4EFD}" name="$CDC: RAGGRUPPAMENTI_adj" dataDxfId="8"/>
+    <tableColumn id="1" xr3:uid="{DB9DB5AC-9FF8-4926-8033-21AB8F0B4EFD}" name="$CDC: RAGGRUPPAMENTI_adj" dataDxfId="10"/>
     <tableColumn id="2" xr3:uid="{06FBF0B0-A15D-4AFB-B465-7242820CF73D}" name="$CON: UNLG - Liv. 2"/>
-    <tableColumn id="4" xr3:uid="{794FE058-6F00-44B3-9FCF-51AA95F79206}" name="Trascodifica" dataDxfId="7"/>
-    <tableColumn id="5" xr3:uid="{DE8BD87C-828E-4931-A2F6-80DEA4839364}" name="Tipo voce" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{794FE058-6F00-44B3-9FCF-51AA95F79206}" name="Trascodifica" dataDxfId="9"/>
+    <tableColumn id="5" xr3:uid="{DE8BD87C-828E-4931-A2F6-80DEA4839364}" name="Tipo voce" dataDxfId="8"/>
     <tableColumn id="6" xr3:uid="{D7A74A4A-9FFA-42A1-A081-4618874B9909}" name="Note"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1356,19 +1384,19 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{18C42134-E9F8-4487-A759-0E0A55C87CC7}" name="Trascodifica_Condizioni_Commerciali" displayName="Trascodifica_Condizioni_Commerciali" ref="A1:C23" totalsRowShown="0" headerRowDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{18C42134-E9F8-4487-A759-0E0A55C87CC7}" name="Trascodifica_Condizioni_Commerciali" displayName="Trascodifica_Condizioni_Commerciali" ref="A1:C23" totalsRowShown="0" headerRowDxfId="7">
   <autoFilter ref="A1:C23" xr:uid="{18C42134-E9F8-4487-A759-0E0A55C87CC7}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{EEC8624E-B158-4B11-8B15-87315EDB7A65}" name="Condizioni commerciali nominali"/>
-    <tableColumn id="2" xr3:uid="{0E26CAB4-E054-46FC-9425-1C33322A5A5F}" name="Condizioni commerciali nominali_riclassificato" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{F50EB424-39EE-40F9-9560-3D7FF968902F}" name="Modalità pagamento" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{0E26CAB4-E054-46FC-9425-1C33322A5A5F}" name="Condizioni commerciali nominali_riclassificato" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{F50EB424-39EE-40F9-9560-3D7FF968902F}" name="Modalità pagamento" dataDxfId="5"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{3A8FC088-1845-4A45-A33F-B35A68332615}" name="Trascodifica_CdC" displayName="Trascodifica_CdC" ref="A1:B13" totalsRowShown="0" headerRowDxfId="2" headerRowCellStyle="Normale 2" dataCellStyle="Normale 2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{3A8FC088-1845-4A45-A33F-B35A68332615}" name="Trascodifica_CdC" displayName="Trascodifica_CdC" ref="A1:B13" totalsRowShown="0" headerRowDxfId="4" headerRowCellStyle="Normale 2" dataCellStyle="Normale 2">
   <autoFilter ref="A1:B13" xr:uid="{3A8FC088-1845-4A45-A33F-B35A68332615}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{7EA54190-3906-4667-AA7A-4FC8279040CA}" name="$CDC: RAGGRUPPAMENTI " dataCellStyle="Normale 2"/>
@@ -1379,11 +1407,23 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{42411417-7B51-4A46-A8D2-79D3CB8FE77A}" name="Trascodifica_Costo_Personale" displayName="Trascodifica_Costo_Personale" ref="A1:B39" totalsRowShown="0" headerRowDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{42411417-7B51-4A46-A8D2-79D3CB8FE77A}" name="Trascodifica_Costo_Personale" displayName="Trascodifica_Costo_Personale" ref="A1:B39" totalsRowShown="0" headerRowDxfId="3">
   <autoFilter ref="A1:B39" xr:uid="{42411417-7B51-4A46-A8D2-79D3CB8FE77A}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{41908B3F-CDCD-4896-B2C7-8E40BD4D38AA}" name="$CON: Codice e descrizione"/>
-    <tableColumn id="2" xr3:uid="{1BD768D9-BD65-4B3D-B940-62522AAB9168}" name="Tipo costo" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{1BD768D9-BD65-4B3D-B940-62522AAB9168}" name="Tipo costo" dataDxfId="2"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{6037E78A-6D25-4BB8-9131-636F1CB5C711}" name="Top_Clienti8" displayName="Top_Clienti8" ref="A1:C11" totalsRowShown="0" headerRowDxfId="1">
+  <autoFilter ref="A1:C11" xr:uid="{6037E78A-6D25-4BB8-9131-636F1CB5C711}"/>
+  <tableColumns count="3">
+    <tableColumn id="4" xr3:uid="{D34D02B1-4924-48FC-A4E2-947D294E5FDB}" name="Soggetto" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{E5C0C14E-D380-48BD-BCB2-5FA0FA6F85AC}" name="Descrizione"/>
+    <tableColumn id="3" xr3:uid="{6C4CADF5-2419-419A-9A00-91121D9DD34E}" name="Tipo cliente"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1692,14 +1732,14 @@
       <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="35.73046875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.9296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
         <v>167</v>
       </c>
@@ -1710,7 +1750,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="13">
         <v>17</v>
       </c>
@@ -1721,7 +1761,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="13">
         <v>25</v>
       </c>
@@ -1732,7 +1772,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="13">
         <v>40</v>
       </c>
@@ -1743,7 +1783,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="13">
         <v>78</v>
       </c>
@@ -1754,7 +1794,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="13">
         <v>79</v>
       </c>
@@ -1765,7 +1805,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="13">
         <v>81</v>
       </c>
@@ -1776,7 +1816,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="13">
         <v>83</v>
       </c>
@@ -1787,7 +1827,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="13">
         <v>84</v>
       </c>
@@ -1798,7 +1838,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="13">
         <v>89</v>
       </c>
@@ -1809,7 +1849,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="13">
         <v>92</v>
       </c>
@@ -1820,7 +1860,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="13">
         <v>93</v>
       </c>
@@ -1831,7 +1871,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="13">
         <v>95</v>
       </c>
@@ -1842,7 +1882,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="13">
         <v>98</v>
       </c>
@@ -1853,7 +1893,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="13">
         <v>99</v>
       </c>
@@ -1864,7 +1904,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="13">
         <v>102</v>
       </c>
@@ -1875,7 +1915,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="13">
         <v>104</v>
       </c>
@@ -1886,7 +1926,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="13">
         <v>105</v>
       </c>
@@ -1897,7 +1937,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="13">
         <v>118</v>
       </c>
@@ -1908,7 +1948,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="13">
         <v>121</v>
       </c>
@@ -1919,7 +1959,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="13">
         <v>122</v>
       </c>
@@ -1930,7 +1970,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="13">
         <v>128</v>
       </c>
@@ -1941,7 +1981,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="13">
         <v>139</v>
       </c>
@@ -1952,7 +1992,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="13">
         <v>141</v>
       </c>
@@ -1963,7 +2003,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="13">
         <v>145</v>
       </c>
@@ -1974,7 +2014,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="13">
         <v>146</v>
       </c>
@@ -1985,7 +2025,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="13">
         <v>147</v>
       </c>
@@ -1996,7 +2036,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="13">
         <v>150</v>
       </c>
@@ -2007,7 +2047,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" s="13">
         <v>160</v>
       </c>
@@ -2018,7 +2058,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" s="13">
         <v>164</v>
       </c>
@@ -2029,7 +2069,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" s="13">
         <v>178</v>
       </c>
@@ -2040,7 +2080,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" s="13">
         <v>182</v>
       </c>
@@ -2051,7 +2091,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" s="13">
         <v>210</v>
       </c>
@@ -2062,7 +2102,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" s="13">
         <v>220</v>
       </c>
@@ -2073,7 +2113,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" s="13">
         <v>228</v>
       </c>
@@ -2084,7 +2124,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" s="13">
         <v>235</v>
       </c>
@@ -2095,7 +2135,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" s="13">
         <v>245</v>
       </c>
@@ -2106,7 +2146,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" s="13">
         <v>250</v>
       </c>
@@ -2117,7 +2157,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" s="13">
         <v>256</v>
       </c>
@@ -2128,7 +2168,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" s="13">
         <v>263</v>
       </c>
@@ -2139,7 +2179,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" s="13">
         <v>272</v>
       </c>
@@ -2150,7 +2190,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" s="13">
         <v>278</v>
       </c>
@@ -2161,7 +2201,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" s="13">
         <v>290</v>
       </c>
@@ -2172,7 +2212,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" s="13">
         <v>291</v>
       </c>
@@ -2183,7 +2223,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" s="13">
         <v>292</v>
       </c>
@@ -2194,7 +2234,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" s="13">
         <v>298</v>
       </c>
@@ -2205,7 +2245,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" s="13">
         <v>299</v>
       </c>
@@ -2225,13 +2265,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1868E1ED-CAEF-4CF4-8725-DD393E3F7908}">
   <dimension ref="A1:C41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+    <sheetView topLeftCell="A8" workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
         <v>167</v>
       </c>
@@ -2242,7 +2282,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="13">
         <v>25</v>
       </c>
@@ -2253,7 +2293,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="13">
         <v>78</v>
       </c>
@@ -2264,7 +2304,7 @@
         <v>0.22000009640349694</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="13">
         <v>79</v>
       </c>
@@ -2275,7 +2315,7 @@
         <v>0.22000000233362949</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="13">
         <v>83</v>
       </c>
@@ -2286,7 +2326,7 @@
         <v>0.21999999999999997</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="13">
         <v>84</v>
       </c>
@@ -2297,7 +2337,7 @@
         <v>0.21999189882532955</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="13">
         <v>89</v>
       </c>
@@ -2308,7 +2348,7 @@
         <v>0.21983125793534719</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="13">
         <v>92</v>
       </c>
@@ -2319,7 +2359,7 @@
         <v>0.22000005397585487</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="13">
         <v>93</v>
       </c>
@@ -2330,7 +2370,7 @@
         <v>0.22</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="13">
         <v>98</v>
       </c>
@@ -2341,7 +2381,7 @@
         <v>0.21999999999999997</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="13">
         <v>99</v>
       </c>
@@ -2352,7 +2392,7 @@
         <v>0.22000031853437774</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="13">
         <v>102</v>
       </c>
@@ -2363,7 +2403,7 @@
         <v>0.22000007862284221</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="13">
         <v>104</v>
       </c>
@@ -2374,7 +2414,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="13">
         <v>105</v>
       </c>
@@ -2385,7 +2425,7 @@
         <v>0.21999998775740814</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="13">
         <v>118</v>
       </c>
@@ -2396,7 +2436,7 @@
         <v>0.22000002495421644</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="13">
         <v>122</v>
       </c>
@@ -2407,7 +2447,7 @@
         <v>0.21999996233635133</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="13">
         <v>139</v>
       </c>
@@ -2418,7 +2458,7 @@
         <v>0.21999999999999997</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="13">
         <v>141</v>
       </c>
@@ -2429,7 +2469,7 @@
         <v>0.22000000791788321</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="13">
         <v>145</v>
       </c>
@@ -2440,7 +2480,7 @@
         <v>0.21999999999999997</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="13">
         <v>146</v>
       </c>
@@ -2451,7 +2491,7 @@
         <v>0.22000014950084057</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="13">
         <v>147</v>
       </c>
@@ -2462,7 +2502,7 @@
         <v>0.21999997759842715</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="13">
         <v>150</v>
       </c>
@@ -2473,7 +2513,7 @@
         <v>0.22000017095110525</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="13">
         <v>160</v>
       </c>
@@ -2484,7 +2524,7 @@
         <v>0.22000005884402474</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="13">
         <v>164</v>
       </c>
@@ -2495,7 +2535,7 @@
         <v>0.21712438709677429</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="13">
         <v>178</v>
       </c>
@@ -2506,7 +2546,7 @@
         <v>1.8906838075475774E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="13">
         <v>182</v>
       </c>
@@ -2517,7 +2557,7 @@
         <v>0.22000004861815081</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="13">
         <v>210</v>
       </c>
@@ -2528,7 +2568,7 @@
         <v>0.21999992342585073</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="13">
         <v>220</v>
       </c>
@@ -2539,7 +2579,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" s="13">
         <v>228</v>
       </c>
@@ -2550,7 +2590,7 @@
         <v>0.2200001696676368</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" s="13">
         <v>235</v>
       </c>
@@ -2561,7 +2601,7 @@
         <v>0.21999999999999997</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" s="13">
         <v>245</v>
       </c>
@@ -2572,7 +2612,7 @@
         <v>0.21999999188952324</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" s="13">
         <v>250</v>
       </c>
@@ -2583,7 +2623,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" s="13">
         <v>256</v>
       </c>
@@ -2594,7 +2634,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" s="13">
         <v>263</v>
       </c>
@@ -2605,7 +2645,7 @@
         <v>0.22000004886685165</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" s="13">
         <v>272</v>
       </c>
@@ -2616,7 +2656,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" s="13">
         <v>278</v>
       </c>
@@ -2627,7 +2667,7 @@
         <v>0.21999994762652597</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" s="13">
         <v>290</v>
       </c>
@@ -2638,7 +2678,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" s="13">
         <v>291</v>
       </c>
@@ -2649,7 +2689,7 @@
         <v>0.22000156966182272</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" s="13">
         <v>292</v>
       </c>
@@ -2660,7 +2700,7 @@
         <v>0.2200391544080269</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" s="13">
         <v>298</v>
       </c>
@@ -2671,7 +2711,7 @@
         <v>0.22000004256548644</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" s="13">
         <v>299</v>
       </c>
@@ -2695,9 +2735,9 @@
       <selection sqref="A1:B29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="15" t="s">
         <v>167</v>
       </c>
@@ -2705,7 +2745,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="16">
         <v>1891</v>
       </c>
@@ -2713,7 +2753,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="16">
         <v>1825</v>
       </c>
@@ -2721,7 +2761,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="16">
         <v>488</v>
       </c>
@@ -2729,7 +2769,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="16">
         <v>763</v>
       </c>
@@ -2737,7 +2777,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="16">
         <v>292</v>
       </c>
@@ -2745,7 +2785,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="16">
         <v>272</v>
       </c>
@@ -2753,7 +2793,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="16">
         <v>990</v>
       </c>
@@ -2761,7 +2801,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="16">
         <v>2656</v>
       </c>
@@ -2769,7 +2809,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="16">
         <v>2030</v>
       </c>
@@ -2777,7 +2817,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="16">
         <v>2082</v>
       </c>
@@ -2785,7 +2825,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="16">
         <v>841</v>
       </c>
@@ -2793,7 +2833,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="16">
         <v>250</v>
       </c>
@@ -2801,7 +2841,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="16">
         <v>385</v>
       </c>
@@ -2809,7 +2849,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="16">
         <v>381</v>
       </c>
@@ -2817,7 +2857,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" s="16">
         <v>444</v>
       </c>
@@ -2825,7 +2865,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="16">
         <v>2054</v>
       </c>
@@ -2833,7 +2873,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="16">
         <v>543</v>
       </c>
@@ -2841,7 +2881,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="16">
         <v>104</v>
       </c>
@@ -2849,7 +2889,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="16">
         <v>316</v>
       </c>
@@ -2857,7 +2897,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="16">
         <v>220</v>
       </c>
@@ -2865,7 +2905,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="16">
         <v>2079</v>
       </c>
@@ -2873,7 +2913,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="16">
         <v>290</v>
       </c>
@@ -2881,7 +2921,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" s="16">
         <v>634</v>
       </c>
@@ -2889,7 +2929,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" s="16">
         <v>1406</v>
       </c>
@@ -2897,7 +2937,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" s="16">
         <v>178</v>
       </c>
@@ -2905,7 +2945,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" s="16">
         <v>256</v>
       </c>
@@ -2913,7 +2953,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" s="16">
         <v>712</v>
       </c>
@@ -2921,7 +2961,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" s="16">
         <v>782</v>
       </c>
@@ -2945,12 +2985,12 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="3" max="3" width="17.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>167</v>
       </c>
@@ -2961,7 +3001,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>178</v>
       </c>
@@ -2972,7 +3012,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>634</v>
       </c>
@@ -2983,7 +3023,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>1801</v>
       </c>
@@ -2994,7 +3034,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>485</v>
       </c>
@@ -3005,7 +3045,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>299</v>
       </c>
@@ -3016,7 +3056,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>811</v>
       </c>
@@ -3027,7 +3067,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>1825</v>
       </c>
@@ -3038,7 +3078,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>1667</v>
       </c>
@@ -3049,7 +3089,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>1408</v>
       </c>
@@ -3060,7 +3100,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>1000</v>
       </c>
@@ -3087,17 +3127,17 @@
       <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="49.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="27.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="32.3984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="29.3984375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.796875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="27.3984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="27.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>42</v>
       </c>
@@ -3117,7 +3157,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="str">
         <f t="shared" ref="A2:A65" si="0">+B2&amp;C2</f>
         <v>Deposito3_01020 Deposito</v>
@@ -3135,7 +3175,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="str">
         <f t="shared" si="0"/>
         <v>Deposito3_01030 Affitto</v>
@@ -3153,7 +3193,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="str">
         <f t="shared" si="0"/>
         <v>Deposito3_04010 Costo lavoro dipendente</v>
@@ -3171,7 +3211,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="str">
         <f t="shared" si="0"/>
         <v>Deposito3_04999 Costo lavoro altri costi</v>
@@ -3189,7 +3229,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="str">
         <f t="shared" si="0"/>
         <v>Deposito3_06020 Costi facchinaggio</v>
@@ -3207,7 +3247,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="str">
         <f t="shared" si="0"/>
         <v>Deposito3_06025 Costi movimentazione esterni</v>
@@ -3225,7 +3265,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="str">
         <f t="shared" si="0"/>
         <v>Deposito3_06210 Costi manutenzione</v>
@@ -3243,7 +3283,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="str">
         <f t="shared" si="0"/>
         <v>Deposito3_06220 Altre spese prestazioni</v>
@@ -3261,7 +3301,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="str">
         <f t="shared" si="0"/>
         <v>Deposito3_06240 Assistenza informatica</v>
@@ -3279,7 +3319,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="str">
         <f t="shared" si="0"/>
         <v>Deposito3_06250 Pulizie</v>
@@ -3297,7 +3337,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="str">
         <f t="shared" si="0"/>
         <v>Deposito3_06270 Noleggi</v>
@@ -3315,7 +3355,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="str">
         <f t="shared" si="0"/>
         <v>Deposito3_06290 Locazione</v>
@@ -3333,7 +3373,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="str">
         <f t="shared" si="0"/>
         <v>Deposito3_06300 Smaltimento</v>
@@ -3351,7 +3391,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="str">
         <f t="shared" si="0"/>
         <v>Deposito3_06310 Assicurazioni</v>
@@ -3372,7 +3412,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="str">
         <f t="shared" si="0"/>
         <v>Deposito3_06330 Danni</v>
@@ -3393,7 +3433,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="str">
         <f t="shared" si="0"/>
         <v>Deposito3_06360 Telefonia</v>
@@ -3411,7 +3451,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="str">
         <f t="shared" si="0"/>
         <v>Deposito3_06380 Ammortamenti</v>
@@ -3429,7 +3469,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="str">
         <f t="shared" si="0"/>
         <v>Deposito3_06999 Altri costi</v>
@@ -3447,7 +3487,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="str">
         <f t="shared" si="0"/>
         <v>Deposito3_08100 Altri ricavi</v>
@@ -3465,7 +3505,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" t="str">
         <f t="shared" si="0"/>
         <v>Deposito3_23100 Costi finanziari</v>
@@ -3483,7 +3523,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" t="str">
         <f t="shared" si="0"/>
         <v>Deposito3_26999 Altre partite straordinarie</v>
@@ -3501,7 +3541,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" t="str">
         <f t="shared" si="0"/>
         <v>Deposito3_28100 Risultato controllata</v>
@@ -3519,7 +3559,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" t="str">
         <f t="shared" si="0"/>
         <v>Groupage3_01010 Trasporto</v>
@@ -3537,7 +3577,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" t="str">
         <f t="shared" si="0"/>
         <v>Groupage3_01020 Deposito</v>
@@ -3555,7 +3595,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" t="str">
         <f t="shared" si="0"/>
         <v>Groupage3_01030 Affitto</v>
@@ -3573,7 +3613,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" t="str">
         <f t="shared" si="0"/>
         <v>Groupage3_01099 Altri ricavi</v>
@@ -3591,7 +3631,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" t="str">
         <f t="shared" si="0"/>
         <v>Groupage3_04010 Costo lavoro dipendente</v>
@@ -3609,7 +3649,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" t="str">
         <f t="shared" si="0"/>
         <v>Groupage3_04999 Costo lavoro altri costi</v>
@@ -3627,7 +3667,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" t="str">
         <f t="shared" si="0"/>
         <v>Groupage3_06010 Costi trasporto</v>
@@ -3645,7 +3685,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" t="str">
         <f t="shared" si="0"/>
         <v>Groupage3_06020 Costi facchinaggio</v>
@@ -3663,7 +3703,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" t="str">
         <f t="shared" si="0"/>
         <v>Groupage3_06025 Costi movimentazione esterni</v>
@@ -3681,7 +3721,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" t="str">
         <f t="shared" si="0"/>
         <v>Groupage3_06030 Carico scarico automezzi</v>
@@ -3699,7 +3739,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" t="str">
         <f t="shared" si="0"/>
         <v>Groupage3_06040 Pallet</v>
@@ -3717,7 +3757,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" t="str">
         <f t="shared" si="0"/>
         <v>Groupage3_06210 Costi manutenzione</v>
@@ -3735,7 +3775,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" t="str">
         <f t="shared" si="0"/>
         <v>Groupage3_06220 Altre spese prestazioni</v>
@@ -3753,7 +3793,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" t="str">
         <f t="shared" si="0"/>
         <v>Groupage3_06240 Assistenza informatica</v>
@@ -3771,7 +3811,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" t="str">
         <f t="shared" si="0"/>
         <v>Groupage3_06250 Pulizie</v>
@@ -3789,7 +3829,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" t="str">
         <f t="shared" si="0"/>
         <v>Groupage3_06260 Vigilanza</v>
@@ -3807,7 +3847,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" t="str">
         <f t="shared" si="0"/>
         <v>Groupage3_06270 Noleggi</v>
@@ -3825,7 +3865,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" t="str">
         <f t="shared" si="0"/>
         <v>Groupage3_06280 Utenze</v>
@@ -3843,7 +3883,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" t="str">
         <f t="shared" si="0"/>
         <v>Groupage3_06290 Locazione</v>
@@ -3864,7 +3904,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" t="str">
         <f t="shared" si="0"/>
         <v>Groupage3_06300 Smaltimento</v>
@@ -3882,7 +3922,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" t="str">
         <f t="shared" si="0"/>
         <v>Groupage3_06310 Assicurazioni</v>
@@ -3903,7 +3943,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" t="str">
         <f t="shared" si="0"/>
         <v>Groupage3_06320 Materiale</v>
@@ -3921,7 +3961,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" t="str">
         <f t="shared" si="0"/>
         <v>Groupage3_06330 Danni</v>
@@ -3942,7 +3982,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" t="str">
         <f t="shared" si="0"/>
         <v>Groupage3_06350 Consulenze/Legali/Sicurezza</v>
@@ -3960,7 +4000,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" t="str">
         <f t="shared" si="0"/>
         <v>Groupage3_06360 Telefonia</v>
@@ -3978,7 +4018,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" t="str">
         <f t="shared" si="0"/>
         <v>Groupage3_06380 Ammortamenti</v>
@@ -3996,7 +4036,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" t="str">
         <f t="shared" si="0"/>
         <v>Groupage3_06999 Altri costi</v>
@@ -4014,7 +4054,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" t="str">
         <f t="shared" si="0"/>
         <v>Groupage3_08100 Altri ricavi</v>
@@ -4032,7 +4072,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" t="str">
         <f t="shared" si="0"/>
         <v>Groupage3_23100 Costi finanziari</v>
@@ -4050,7 +4090,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" t="str">
         <f t="shared" si="0"/>
         <v>Groupage3_26999 Altre partite straordinarie</v>
@@ -4068,7 +4108,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" t="str">
         <f t="shared" si="0"/>
         <v>Groupage3_28100 Risultato controllata</v>
@@ -4086,7 +4126,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" t="str">
         <f t="shared" si="0"/>
         <v>Groupage3_29100 Imposte tasse comunali/CCIAA</v>
@@ -4104,7 +4144,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56" t="str">
         <f t="shared" si="0"/>
         <v>Trasporto3_01010 Trasporto</v>
@@ -4122,7 +4162,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57" t="str">
         <f t="shared" si="0"/>
         <v>Trasporto3_04010 Costo lavoro dipendente</v>
@@ -4140,7 +4180,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58" t="str">
         <f t="shared" si="0"/>
         <v>Trasporto3_04999 Costo lavoro altri costi</v>
@@ -4158,7 +4198,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59" t="str">
         <f t="shared" si="0"/>
         <v>Trasporto3_06010 Costi trasporto</v>
@@ -4176,7 +4216,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A60" t="str">
         <f t="shared" si="0"/>
         <v>Trasporto3_06020 Costi facchinaggio</v>
@@ -4194,7 +4234,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A61" t="str">
         <f t="shared" si="0"/>
         <v>Trasporto3_06025 Costi movimentazione esterni</v>
@@ -4212,7 +4252,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A62" t="str">
         <f t="shared" si="0"/>
         <v>Trasporto3_06210 Costi manutenzione</v>
@@ -4230,7 +4270,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A63" t="str">
         <f t="shared" si="0"/>
         <v>Trasporto3_06220 Altre spese prestazioni</v>
@@ -4248,7 +4288,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A64" t="str">
         <f t="shared" si="0"/>
         <v>Trasporto3_06240 Assistenza informatica</v>
@@ -4266,7 +4306,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A65" t="str">
         <f t="shared" si="0"/>
         <v>Trasporto3_06250 Pulizie</v>
@@ -4284,7 +4324,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A66" t="str">
         <f t="shared" ref="A66:A108" si="1">+B66&amp;C66</f>
         <v>Trasporto3_06270 Noleggi</v>
@@ -4302,7 +4342,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A67" t="str">
         <f t="shared" si="1"/>
         <v>Trasporto3_06310 Assicurazioni</v>
@@ -4323,7 +4363,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A68" t="str">
         <f t="shared" si="1"/>
         <v>Trasporto3_06320 Materiale</v>
@@ -4341,7 +4381,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A69" t="str">
         <f t="shared" si="1"/>
         <v>Trasporto3_06330 Danni</v>
@@ -4362,7 +4402,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A70" t="str">
         <f t="shared" si="1"/>
         <v>Trasporto3_06360 Telefonia</v>
@@ -4380,7 +4420,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A71" t="str">
         <f t="shared" si="1"/>
         <v>Trasporto3_06380 Ammortamenti</v>
@@ -4398,7 +4438,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A72" t="str">
         <f t="shared" si="1"/>
         <v>Trasporto3_06999 Altri costi</v>
@@ -4416,7 +4456,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A73" t="str">
         <f t="shared" si="1"/>
         <v>Trasporto3_08100 Altri ricavi</v>
@@ -4434,7 +4474,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A74" t="str">
         <f t="shared" si="1"/>
         <v>Trasporto3_23100 Costi finanziari</v>
@@ -4452,7 +4492,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A75" t="str">
         <f t="shared" si="1"/>
         <v>Trasporto3_26999 Altre partite straordinarie</v>
@@ -4470,7 +4510,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A76" t="str">
         <f t="shared" si="1"/>
         <v>Ricavi / Costi indiretti3_01010 Trasporto</v>
@@ -4488,7 +4528,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A77" t="str">
         <f t="shared" si="1"/>
         <v>Ricavi / Costi indiretti3_04010 Costo lavoro dipendente</v>
@@ -4506,7 +4546,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A78" t="str">
         <f t="shared" si="1"/>
         <v>Ricavi / Costi indiretti3_04999 Costo lavoro altri costi</v>
@@ -4524,7 +4564,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A79" t="str">
         <f t="shared" si="1"/>
         <v>Ricavi / Costi indiretti3_06210 Costi manutenzione</v>
@@ -4542,7 +4582,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A80" t="str">
         <f t="shared" si="1"/>
         <v>Ricavi / Costi indiretti3_06220 Altre spese prestazioni</v>
@@ -4560,7 +4600,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A81" t="str">
         <f t="shared" si="1"/>
         <v>Ricavi / Costi indiretti3_06240 Assistenza informatica</v>
@@ -4578,7 +4618,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A82" t="str">
         <f t="shared" si="1"/>
         <v>Ricavi / Costi indiretti3_06250 Pulizie</v>
@@ -4596,7 +4636,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A83" t="str">
         <f t="shared" si="1"/>
         <v>Ricavi / Costi indiretti3_06260 Vigilanza</v>
@@ -4614,7 +4654,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A84" t="str">
         <f t="shared" si="1"/>
         <v>Ricavi / Costi indiretti3_06270 Noleggi</v>
@@ -4632,7 +4672,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A85" t="str">
         <f t="shared" si="1"/>
         <v>Ricavi / Costi indiretti3_06280 Utenze</v>
@@ -4650,7 +4690,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A86" t="str">
         <f t="shared" si="1"/>
         <v>Ricavi / Costi indiretti3_06290 Locazione</v>
@@ -4668,7 +4708,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A87" t="str">
         <f t="shared" si="1"/>
         <v>Ricavi / Costi indiretti3_06310 Assicurazioni</v>
@@ -4686,7 +4726,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A88" t="str">
         <f t="shared" si="1"/>
         <v>Ricavi / Costi indiretti3_06320 Materiale</v>
@@ -4704,7 +4744,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A89" t="str">
         <f t="shared" si="1"/>
         <v>Ricavi / Costi indiretti3_06350 Consulenze/Legali/Sicurezza</v>
@@ -4722,7 +4762,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A90" t="str">
         <f t="shared" si="1"/>
         <v>Ricavi / Costi indiretti3_06360 Telefonia</v>
@@ -4740,7 +4780,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A91" t="str">
         <f t="shared" si="1"/>
         <v>Ricavi / Costi indiretti3_06370 Pubblicità</v>
@@ -4758,7 +4798,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A92" t="str">
         <f t="shared" si="1"/>
         <v>Ricavi / Costi indiretti3_06380 Ammortamenti</v>
@@ -4776,7 +4816,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A93" t="str">
         <f t="shared" si="1"/>
         <v>Ricavi / Costi indiretti3_06999 Altri costi</v>
@@ -4794,7 +4834,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A94" t="str">
         <f t="shared" si="1"/>
         <v>Ricavi / Costi indiretti3_08100 Altri ricavi</v>
@@ -4812,7 +4852,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A95" t="str">
         <f t="shared" si="1"/>
         <v>Ricavi / Costi indiretti3_23100 Costi finanziari</v>
@@ -4830,7 +4870,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A96" t="str">
         <f t="shared" si="1"/>
         <v>Ricavi / Costi indiretti3_26999 Altre partite straordinarie</v>
@@ -4848,7 +4888,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A97" t="str">
         <f t="shared" si="1"/>
         <v>Ricavi / Costi indiretti3_29100 Imposte tasse comunali/CCIAA</v>
@@ -4866,7 +4906,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A98" t="str">
         <f t="shared" si="1"/>
         <v>Ricavi / Costi indiretti3_59100 Costi societari</v>
@@ -4884,7 +4924,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A99" t="str">
         <f t="shared" si="1"/>
         <v>Ricavi / Costi indiretti3_70100 Accantonamenti</v>
@@ -4902,7 +4942,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A100" t="str">
         <f t="shared" si="1"/>
         <v>Ricavi / Costi indiretti3_90100 Imposte tasse sul reddito</v>
@@ -4920,7 +4960,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A101" t="str">
         <f t="shared" si="1"/>
         <v>Groupage3_04030 Costo lavoro collaboratori</v>
@@ -4938,7 +4978,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A102" t="str">
         <f t="shared" si="1"/>
         <v>Deposito3_06320 Materiale</v>
@@ -4956,7 +4996,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A103" t="str">
         <f t="shared" si="1"/>
         <v>Ricavi / Costi indiretti3_04030 Costo lavoro collaboratori</v>
@@ -4974,7 +5014,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A104" t="str">
         <f t="shared" si="1"/>
         <v>Trasporto3_06350 Consulenze/Legali/Sicurezza</v>
@@ -4992,7 +5032,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A105" t="str">
         <f t="shared" si="1"/>
         <v>Deposito3_06350 Consulenze/Legali/Sicurezza</v>
@@ -5010,7 +5050,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A106" t="str">
         <f t="shared" si="1"/>
         <v>Groupage3_80100 Utilizzo Fondi Rischi</v>
@@ -5028,7 +5068,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A107" t="str">
         <f t="shared" si="1"/>
         <v>Trasporto3_80100 Utilizzo Fondi Rischi</v>
@@ -5046,7 +5086,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A108" t="str">
         <f t="shared" si="1"/>
         <v>Ricavi / Costi indiretti3_80100 Utilizzo Fondi Rischi</v>
@@ -5080,12 +5120,12 @@
       <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="24.796875" customWidth="1"/>
+    <col min="2" max="2" width="24.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>121</v>
       </c>
@@ -5096,7 +5136,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>124</v>
       </c>
@@ -5107,7 +5147,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>127</v>
       </c>
@@ -5118,7 +5158,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>130</v>
       </c>
@@ -5129,7 +5169,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>131</v>
       </c>
@@ -5140,7 +5180,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>133</v>
       </c>
@@ -5151,7 +5191,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>134</v>
       </c>
@@ -5162,7 +5202,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>135</v>
       </c>
@@ -5173,7 +5213,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>136</v>
       </c>
@@ -5184,7 +5224,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>138</v>
       </c>
@@ -5195,7 +5235,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>139</v>
       </c>
@@ -5206,7 +5246,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>140</v>
       </c>
@@ -5217,7 +5257,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>141</v>
       </c>
@@ -5228,7 +5268,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>142</v>
       </c>
@@ -5239,7 +5279,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>143</v>
       </c>
@@ -5250,7 +5290,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>144</v>
       </c>
@@ -5261,7 +5301,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>145</v>
       </c>
@@ -5272,7 +5312,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>146</v>
       </c>
@@ -5283,7 +5323,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>147</v>
       </c>
@@ -5294,7 +5334,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>148</v>
       </c>
@@ -5305,7 +5345,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>149</v>
       </c>
@@ -5316,7 +5356,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>151</v>
       </c>
@@ -5327,7 +5367,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>152</v>
       </c>
@@ -5354,13 +5394,13 @@
       <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="28.59765625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>153</v>
       </c>
@@ -5368,7 +5408,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
         <v>155</v>
       </c>
@@ -5376,7 +5416,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
         <v>156</v>
       </c>
@@ -5384,7 +5424,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
         <v>157</v>
       </c>
@@ -5392,7 +5432,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
         <v>158</v>
       </c>
@@ -5400,7 +5440,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="8" t="s">
         <v>159</v>
       </c>
@@ -5408,7 +5448,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="8" t="s">
         <v>160</v>
       </c>
@@ -5416,7 +5456,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="9" t="s">
         <v>161</v>
       </c>
@@ -5424,7 +5464,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="8" t="s">
         <v>162</v>
       </c>
@@ -5432,7 +5472,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="8" t="s">
         <v>163</v>
       </c>
@@ -5440,7 +5480,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="8" t="s">
         <v>164</v>
       </c>
@@ -5448,7 +5488,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="8" t="s">
         <v>165</v>
       </c>
@@ -5456,7 +5496,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="8" t="s">
         <v>166</v>
       </c>
@@ -5480,13 +5520,13 @@
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="41.3984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.73046875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="41.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5494,7 +5534,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -5502,7 +5542,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -5510,7 +5550,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -5518,7 +5558,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -5526,7 +5566,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -5534,7 +5574,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -5542,7 +5582,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -5550,7 +5590,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -5558,7 +5598,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -5566,7 +5606,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -5574,7 +5614,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>14</v>
       </c>
@@ -5582,7 +5622,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>15</v>
       </c>
@@ -5590,7 +5630,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>16</v>
       </c>
@@ -5598,7 +5638,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>17</v>
       </c>
@@ -5606,7 +5646,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>18</v>
       </c>
@@ -5614,7 +5654,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>19</v>
       </c>
@@ -5622,7 +5662,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>20</v>
       </c>
@@ -5630,7 +5670,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>21</v>
       </c>
@@ -5638,7 +5678,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>22</v>
       </c>
@@ -5646,7 +5686,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>23</v>
       </c>
@@ -5654,7 +5694,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>24</v>
       </c>
@@ -5662,7 +5702,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>25</v>
       </c>
@@ -5670,7 +5710,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>26</v>
       </c>
@@ -5678,7 +5718,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>27</v>
       </c>
@@ -5686,7 +5726,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>28</v>
       </c>
@@ -5694,7 +5734,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>29</v>
       </c>
@@ -5702,7 +5742,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>30</v>
       </c>
@@ -5710,7 +5750,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>31</v>
       </c>
@@ -5718,7 +5758,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>32</v>
       </c>
@@ -5726,7 +5766,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>33</v>
       </c>
@@ -5734,7 +5774,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>34</v>
       </c>
@@ -5742,7 +5782,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>35</v>
       </c>
@@ -5750,7 +5790,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>36</v>
       </c>
@@ -5758,7 +5798,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>37</v>
       </c>
@@ -5766,7 +5806,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>38</v>
       </c>
@@ -5774,7 +5814,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>39</v>
       </c>
@@ -5782,7 +5822,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>40</v>
       </c>
@@ -5790,12 +5830,151 @@
         <v>3</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>41</v>
       </c>
       <c r="B39" s="2" t="s">
         <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF4B4923-26BF-4B6C-8210-10F46399C135}">
+  <dimension ref="A1:C11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:C11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>178</v>
+      </c>
+      <c r="B2" t="s">
+        <v>170</v>
+      </c>
+      <c r="C2" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>634</v>
+      </c>
+      <c r="B3" t="s">
+        <v>172</v>
+      </c>
+      <c r="C3" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>1801</v>
+      </c>
+      <c r="B4" t="s">
+        <v>173</v>
+      </c>
+      <c r="C4" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>485</v>
+      </c>
+      <c r="B5" t="s">
+        <v>174</v>
+      </c>
+      <c r="C5" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>299</v>
+      </c>
+      <c r="B6" t="s">
+        <v>175</v>
+      </c>
+      <c r="C6" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>811</v>
+      </c>
+      <c r="B7" t="s">
+        <v>176</v>
+      </c>
+      <c r="C7" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>1825</v>
+      </c>
+      <c r="B8" t="s">
+        <v>177</v>
+      </c>
+      <c r="C8" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>1667</v>
+      </c>
+      <c r="B9" t="s">
+        <v>178</v>
+      </c>
+      <c r="C9" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>1408</v>
+      </c>
+      <c r="B10" t="s">
+        <v>180</v>
+      </c>
+      <c r="C10" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>1000</v>
+      </c>
+      <c r="B11" t="s">
+        <v>181</v>
+      </c>
+      <c r="C11" t="s">
+        <v>171</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Cancella modifiche inutili a support_trascodifiche
</commit_message>
<xml_diff>
--- a/inputs/support_trascodifiche.xlsx
+++ b/inputs/support_trascodifiche.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LUP\Documents\GitHub\22p11_Tool_FA\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0ADF50D-AE1A-4303-89FF-2A5DF8522C7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11EC0C41-93D7-423D-9F37-992A42D84B80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" firstSheet="5" activeTab="8" xr2:uid="{9758A490-5BBA-4DAE-A128-35FF12EB83CB}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" firstSheet="3" activeTab="3" xr2:uid="{9758A490-5BBA-4DAE-A128-35FF12EB83CB}"/>
   </bookViews>
   <sheets>
     <sheet name="Condizioni_Commerciali" sheetId="7" r:id="rId1"/>
@@ -21,7 +21,6 @@
     <sheet name="Trascodifica_Condizioni_comm_li" sheetId="3" r:id="rId6"/>
     <sheet name="Trascodifica_CdC" sheetId="4" r:id="rId7"/>
     <sheet name="Trascodifica_Costo_Personale" sheetId="1" r:id="rId8"/>
-    <sheet name="Top_clienti" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -43,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="828" uniqueCount="253">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="805" uniqueCount="253">
   <si>
     <t>$CON: Codice e descrizione</t>
   </si>
@@ -1016,34 +1015,7 @@
     <cellStyle name="Normale 2" xfId="1" xr:uid="{3D0E86AB-4D3C-45D0-B0FD-4FA2CF8A5195}"/>
     <cellStyle name="Normale 7" xfId="2" xr:uid="{53EBC274-2193-4F8D-84F3-098F077B8327}"/>
   </cellStyles>
-  <dxfs count="17">
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="0"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="15">
     <dxf>
       <font>
         <b val="0"/>
@@ -1344,10 +1316,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{A4B5F73C-8C81-4BA0-9486-D78D8D2EDA32}" name="Elenco_Esportatori" displayName="Elenco_Esportatori" ref="A1:B29" totalsRowShown="0" headerRowDxfId="16" headerRowCellStyle="Normale 7" dataCellStyle="Normale 7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{A4B5F73C-8C81-4BA0-9486-D78D8D2EDA32}" name="Elenco_Esportatori" displayName="Elenco_Esportatori" ref="A1:B29" totalsRowShown="0" headerRowDxfId="14" headerRowCellStyle="Normale 7" dataCellStyle="Normale 7">
   <autoFilter ref="A1:B29" xr:uid="{A4B5F73C-8C81-4BA0-9486-D78D8D2EDA32}"/>
   <tableColumns count="2">
-    <tableColumn id="3" xr3:uid="{B1F89080-23D9-46D2-A0A2-ECC915269C09}" name="Soggetto" dataDxfId="15" dataCellStyle="Normale 7"/>
+    <tableColumn id="3" xr3:uid="{B1F89080-23D9-46D2-A0A2-ECC915269C09}" name="Soggetto" dataDxfId="13" dataCellStyle="Normale 7"/>
     <tableColumn id="2" xr3:uid="{6CE5CCEB-2876-4548-B4E6-7A22BC4AC5CA}" name="Ter_descr" dataCellStyle="Normale 7"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1355,10 +1327,10 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{A4CD4984-42E8-4E8F-9C29-4F867B1919A0}" name="Top_Clienti" displayName="Top_Clienti" ref="A1:C11" totalsRowShown="0" headerRowDxfId="14">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{A4CD4984-42E8-4E8F-9C29-4F867B1919A0}" name="Top_Clienti" displayName="Top_Clienti" ref="A1:C11" totalsRowShown="0" headerRowDxfId="12">
   <autoFilter ref="A1:C11" xr:uid="{A4CD4984-42E8-4E8F-9C29-4F867B1919A0}"/>
   <tableColumns count="3">
-    <tableColumn id="4" xr3:uid="{6AAC45EB-A00C-459D-8C5B-AC959ABE7DCD}" name="Soggetto" dataDxfId="13"/>
+    <tableColumn id="4" xr3:uid="{6AAC45EB-A00C-459D-8C5B-AC959ABE7DCD}" name="Soggetto" dataDxfId="11"/>
     <tableColumn id="2" xr3:uid="{7B6BFE59-FA92-466B-995F-DD6BD01640AB}" name="Descrizione"/>
     <tableColumn id="3" xr3:uid="{2088016D-F766-4701-8F36-DF5294CD2639}" name="Tipo cliente"/>
   </tableColumns>
@@ -1367,16 +1339,16 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{E832CCEC-F5F5-42D8-8383-1933DC5C8C1D}" name="Trascodifica_Analitico_CE" displayName="Trascodifica_Analitico_CE" ref="A1:F108" totalsRowShown="0" headerRowDxfId="12">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{E832CCEC-F5F5-42D8-8383-1933DC5C8C1D}" name="Trascodifica_Analitico_CE" displayName="Trascodifica_Analitico_CE" ref="A1:F108" totalsRowShown="0" headerRowDxfId="10">
   <autoFilter ref="A1:F108" xr:uid="{E832CCEC-F5F5-42D8-8383-1933DC5C8C1D}"/>
   <tableColumns count="6">
-    <tableColumn id="3" xr3:uid="{EDD3DE90-20FA-4C95-8697-6D0CFBD3D34A}" name="Chiave trascodifica" dataDxfId="11">
+    <tableColumn id="3" xr3:uid="{EDD3DE90-20FA-4C95-8697-6D0CFBD3D34A}" name="Chiave trascodifica" dataDxfId="9">
       <calculatedColumnFormula>+B2&amp;C2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="1" xr3:uid="{DB9DB5AC-9FF8-4926-8033-21AB8F0B4EFD}" name="$CDC: RAGGRUPPAMENTI_adj" dataDxfId="10"/>
+    <tableColumn id="1" xr3:uid="{DB9DB5AC-9FF8-4926-8033-21AB8F0B4EFD}" name="$CDC: RAGGRUPPAMENTI_adj" dataDxfId="8"/>
     <tableColumn id="2" xr3:uid="{06FBF0B0-A15D-4AFB-B465-7242820CF73D}" name="$CON: UNLG - Liv. 2"/>
-    <tableColumn id="4" xr3:uid="{794FE058-6F00-44B3-9FCF-51AA95F79206}" name="Trascodifica" dataDxfId="9"/>
-    <tableColumn id="5" xr3:uid="{DE8BD87C-828E-4931-A2F6-80DEA4839364}" name="Tipo voce" dataDxfId="8"/>
+    <tableColumn id="4" xr3:uid="{794FE058-6F00-44B3-9FCF-51AA95F79206}" name="Trascodifica" dataDxfId="7"/>
+    <tableColumn id="5" xr3:uid="{DE8BD87C-828E-4931-A2F6-80DEA4839364}" name="Tipo voce" dataDxfId="6"/>
     <tableColumn id="6" xr3:uid="{D7A74A4A-9FFA-42A1-A081-4618874B9909}" name="Note"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1384,19 +1356,19 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{18C42134-E9F8-4487-A759-0E0A55C87CC7}" name="Trascodifica_Condizioni_Commerciali" displayName="Trascodifica_Condizioni_Commerciali" ref="A1:C23" totalsRowShown="0" headerRowDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{18C42134-E9F8-4487-A759-0E0A55C87CC7}" name="Trascodifica_Condizioni_Commerciali" displayName="Trascodifica_Condizioni_Commerciali" ref="A1:C23" totalsRowShown="0" headerRowDxfId="5">
   <autoFilter ref="A1:C23" xr:uid="{18C42134-E9F8-4487-A759-0E0A55C87CC7}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{EEC8624E-B158-4B11-8B15-87315EDB7A65}" name="Condizioni commerciali nominali"/>
-    <tableColumn id="2" xr3:uid="{0E26CAB4-E054-46FC-9425-1C33322A5A5F}" name="Condizioni commerciali nominali_riclassificato" dataDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{F50EB424-39EE-40F9-9560-3D7FF968902F}" name="Modalità pagamento" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{0E26CAB4-E054-46FC-9425-1C33322A5A5F}" name="Condizioni commerciali nominali_riclassificato" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{F50EB424-39EE-40F9-9560-3D7FF968902F}" name="Modalità pagamento" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{3A8FC088-1845-4A45-A33F-B35A68332615}" name="Trascodifica_CdC" displayName="Trascodifica_CdC" ref="A1:B13" totalsRowShown="0" headerRowDxfId="4" headerRowCellStyle="Normale 2" dataCellStyle="Normale 2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{3A8FC088-1845-4A45-A33F-B35A68332615}" name="Trascodifica_CdC" displayName="Trascodifica_CdC" ref="A1:B13" totalsRowShown="0" headerRowDxfId="2" headerRowCellStyle="Normale 2" dataCellStyle="Normale 2">
   <autoFilter ref="A1:B13" xr:uid="{3A8FC088-1845-4A45-A33F-B35A68332615}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{7EA54190-3906-4667-AA7A-4FC8279040CA}" name="$CDC: RAGGRUPPAMENTI " dataCellStyle="Normale 2"/>
@@ -1407,23 +1379,11 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{42411417-7B51-4A46-A8D2-79D3CB8FE77A}" name="Trascodifica_Costo_Personale" displayName="Trascodifica_Costo_Personale" ref="A1:B39" totalsRowShown="0" headerRowDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{42411417-7B51-4A46-A8D2-79D3CB8FE77A}" name="Trascodifica_Costo_Personale" displayName="Trascodifica_Costo_Personale" ref="A1:B39" totalsRowShown="0" headerRowDxfId="1">
   <autoFilter ref="A1:B39" xr:uid="{42411417-7B51-4A46-A8D2-79D3CB8FE77A}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{41908B3F-CDCD-4896-B2C7-8E40BD4D38AA}" name="$CON: Codice e descrizione"/>
-    <tableColumn id="2" xr3:uid="{1BD768D9-BD65-4B3D-B940-62522AAB9168}" name="Tipo costo" dataDxfId="2"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{6037E78A-6D25-4BB8-9131-636F1CB5C711}" name="Top_Clienti8" displayName="Top_Clienti8" ref="A1:C11" totalsRowShown="0" headerRowDxfId="1">
-  <autoFilter ref="A1:C11" xr:uid="{6037E78A-6D25-4BB8-9131-636F1CB5C711}"/>
-  <tableColumns count="3">
-    <tableColumn id="4" xr3:uid="{D34D02B1-4924-48FC-A4E2-947D294E5FDB}" name="Soggetto" dataDxfId="0"/>
-    <tableColumn id="2" xr3:uid="{E5C0C14E-D380-48BD-BCB2-5FA0FA6F85AC}" name="Descrizione"/>
-    <tableColumn id="3" xr3:uid="{6C4CADF5-2419-419A-9A00-91121D9DD34E}" name="Tipo cliente"/>
+    <tableColumn id="2" xr3:uid="{1BD768D9-BD65-4B3D-B940-62522AAB9168}" name="Tipo costo" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2981,7 +2941,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1108AB1-127A-4D50-9F30-C7486AA9E608}">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -5844,143 +5804,4 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF4B4923-26BF-4B6C-8210-10F46399C135}">
-  <dimension ref="A1:C11"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>178</v>
-      </c>
-      <c r="B2" t="s">
-        <v>170</v>
-      </c>
-      <c r="C2" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>634</v>
-      </c>
-      <c r="B3" t="s">
-        <v>172</v>
-      </c>
-      <c r="C3" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>1801</v>
-      </c>
-      <c r="B4" t="s">
-        <v>173</v>
-      </c>
-      <c r="C4" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>485</v>
-      </c>
-      <c r="B5" t="s">
-        <v>174</v>
-      </c>
-      <c r="C5" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>299</v>
-      </c>
-      <c r="B6" t="s">
-        <v>175</v>
-      </c>
-      <c r="C6" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7">
-        <v>811</v>
-      </c>
-      <c r="B7" t="s">
-        <v>176</v>
-      </c>
-      <c r="C7" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8">
-        <v>1825</v>
-      </c>
-      <c r="B8" t="s">
-        <v>177</v>
-      </c>
-      <c r="C8" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9">
-        <v>1667</v>
-      </c>
-      <c r="B9" t="s">
-        <v>178</v>
-      </c>
-      <c r="C9" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10">
-        <v>1408</v>
-      </c>
-      <c r="B10" t="s">
-        <v>180</v>
-      </c>
-      <c r="C10" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11">
-        <v>1000</v>
-      </c>
-      <c r="B11" t="s">
-        <v>181</v>
-      </c>
-      <c r="C11" t="s">
-        <v>171</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
-</worksheet>
 </file>
</xml_diff>